<commit_message>
fix contract upgrade value was too high for player
</commit_message>
<xml_diff>
--- a/contracts/scripts/GameConfig.xlsx
+++ b/contracts/scripts/GameConfig.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\smart-contract\EthBuildQuest_FadingHope\scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\smart-contract\EthBuildQuest_FadingHope\contracts\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC345F7A-C0E5-4B1A-BBE9-731DE06F9BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A04CD55A-DBE0-4F35-A98B-D05CDF781FE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5520" yWindow="705" windowWidth="21600" windowHeight="11385" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exponential Item Growth" sheetId="1" r:id="rId1"/>
@@ -368,17 +368,17 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="11" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -27666,6 +27666,60 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="AutoShape 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25637131-5AAB-4A5D-9578-3E83D8FAABA7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -28004,17 +28058,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E2" s="3"/>
@@ -54920,7 +54974,7 @@
   <dimension ref="A1:R83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -54978,34 +55032,34 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2" s="23">
+      <c r="A2" s="21">
         <v>0</v>
       </c>
-      <c r="B2" s="24">
+      <c r="B2" s="22">
         <v>0</v>
       </c>
-      <c r="C2" s="24">
+      <c r="C2" s="22">
         <v>1</v>
       </c>
-      <c r="D2" s="25">
+      <c r="D2" s="23">
         <v>0</v>
       </c>
-      <c r="E2" s="25">
+      <c r="E2" s="23">
         <v>0</v>
       </c>
-      <c r="F2" s="25">
+      <c r="F2" s="23">
         <v>0</v>
       </c>
-      <c r="G2" s="25"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="24">
+      <c r="G2" s="23"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="22">
         <v>0</v>
       </c>
-      <c r="N2" s="24">
+      <c r="N2" s="22">
         <v>0</v>
       </c>
       <c r="O2">
@@ -55023,7 +55077,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="16">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="C3" s="16">
         <v>4</v>
@@ -55047,11 +55101,11 @@
       </c>
       <c r="M3" s="16">
         <f>B3*I$5</f>
-        <v>300</v>
+        <v>60</v>
       </c>
       <c r="N3" s="16">
         <f>B3*I$6</f>
-        <v>120</v>
+        <v>24</v>
       </c>
       <c r="O3">
         <v>1000</v>
@@ -55067,7 +55121,7 @@
       </c>
       <c r="B4" s="16">
         <f t="shared" ref="B4:B35" si="0">B3*I$3</f>
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="C4" s="16">
         <v>6</v>
@@ -55088,11 +55142,11 @@
       </c>
       <c r="M4" s="16">
         <f t="shared" ref="M4:M67" si="2">B4*I$5</f>
-        <v>1500</v>
+        <v>300</v>
       </c>
       <c r="N4" s="16">
         <f t="shared" ref="N4:N67" si="3">B4*I$6</f>
-        <v>600</v>
+        <v>120</v>
       </c>
       <c r="Q4">
         <f>Q3*J$11</f>
@@ -55106,11 +55160,11 @@
       </c>
       <c r="B5" s="16">
         <f t="shared" si="0"/>
-        <v>2500</v>
+        <v>500</v>
       </c>
       <c r="C5" s="16">
         <f t="shared" ref="C5:C68" si="5">B5/(D5*3600)</f>
-        <v>13.888888888888889</v>
+        <v>2.7777777777777777</v>
       </c>
       <c r="D5">
         <v>0.05</v>
@@ -55131,11 +55185,11 @@
       </c>
       <c r="M5" s="16">
         <f t="shared" si="2"/>
-        <v>7500</v>
+        <v>1500</v>
       </c>
       <c r="N5" s="16">
         <f t="shared" si="3"/>
-        <v>3000</v>
+        <v>600</v>
       </c>
       <c r="Q5">
         <f t="shared" ref="Q5:Q68" si="7">Q4*J$11</f>
@@ -55149,11 +55203,11 @@
       </c>
       <c r="B6" s="16">
         <f t="shared" si="0"/>
-        <v>12500</v>
+        <v>2500</v>
       </c>
       <c r="C6" s="16">
         <f t="shared" si="5"/>
-        <v>57.870370370370374</v>
+        <v>11.574074074074074</v>
       </c>
       <c r="D6">
         <v>0.06</v>
@@ -55174,11 +55228,11 @@
       </c>
       <c r="M6" s="16">
         <f t="shared" si="2"/>
-        <v>37500</v>
+        <v>7500</v>
       </c>
       <c r="N6" s="16">
         <f t="shared" si="3"/>
-        <v>15000</v>
+        <v>3000</v>
       </c>
       <c r="Q6">
         <f t="shared" si="7"/>
@@ -55192,11 +55246,11 @@
       </c>
       <c r="B7" s="16">
         <f t="shared" si="0"/>
-        <v>62500</v>
+        <v>12500</v>
       </c>
       <c r="C7" s="16">
         <f t="shared" si="5"/>
-        <v>144.67592592592592</v>
+        <v>28.935185185185187</v>
       </c>
       <c r="D7" s="18">
         <f>D6*2</f>
@@ -55212,11 +55266,11 @@
       </c>
       <c r="M7" s="16">
         <f t="shared" si="2"/>
-        <v>187500</v>
+        <v>37500</v>
       </c>
       <c r="N7" s="16">
         <f t="shared" si="3"/>
-        <v>75000</v>
+        <v>15000</v>
       </c>
       <c r="Q7">
         <f t="shared" si="7"/>
@@ -55230,11 +55284,11 @@
       </c>
       <c r="B8" s="16">
         <f t="shared" si="0"/>
-        <v>312500</v>
+        <v>62500</v>
       </c>
       <c r="C8" s="16">
         <f t="shared" si="5"/>
-        <v>361.68981481481484</v>
+        <v>72.337962962962962</v>
       </c>
       <c r="D8" s="18">
         <f>D7*2</f>
@@ -55253,11 +55307,11 @@
       </c>
       <c r="M8" s="16">
         <f t="shared" si="2"/>
-        <v>937500</v>
+        <v>187500</v>
       </c>
       <c r="N8" s="16">
         <f t="shared" si="3"/>
-        <v>375000</v>
+        <v>75000</v>
       </c>
       <c r="Q8">
         <f t="shared" si="7"/>
@@ -55271,11 +55325,11 @@
       </c>
       <c r="B9" s="16">
         <f t="shared" si="0"/>
-        <v>1562500</v>
+        <v>312500</v>
       </c>
       <c r="C9" s="16">
         <f t="shared" si="5"/>
-        <v>904.22453703703707</v>
+        <v>180.84490740740742</v>
       </c>
       <c r="D9" s="18">
         <f t="shared" ref="D9:D11" si="8">D8*2</f>
@@ -55294,11 +55348,11 @@
       </c>
       <c r="M9" s="16">
         <f t="shared" si="2"/>
-        <v>4687500</v>
+        <v>937500</v>
       </c>
       <c r="N9" s="16">
         <f t="shared" si="3"/>
-        <v>1875000</v>
+        <v>375000</v>
       </c>
       <c r="Q9">
         <f t="shared" si="7"/>
@@ -55312,11 +55366,11 @@
       </c>
       <c r="B10" s="16">
         <f t="shared" si="0"/>
-        <v>7812500</v>
+        <v>1562500</v>
       </c>
       <c r="C10" s="16">
         <f t="shared" si="5"/>
-        <v>2260.5613425925926</v>
+        <v>452.11226851851853</v>
       </c>
       <c r="D10" s="18">
         <f t="shared" si="8"/>
@@ -55332,11 +55386,11 @@
       </c>
       <c r="M10" s="16">
         <f t="shared" si="2"/>
-        <v>23437500</v>
+        <v>4687500</v>
       </c>
       <c r="N10" s="16">
         <f t="shared" si="3"/>
-        <v>9375000</v>
+        <v>1875000</v>
       </c>
       <c r="Q10">
         <f t="shared" si="7"/>
@@ -55350,11 +55404,11 @@
       </c>
       <c r="B11" s="16">
         <f t="shared" si="0"/>
-        <v>39062500</v>
+        <v>7812500</v>
       </c>
       <c r="C11" s="16">
         <f t="shared" si="5"/>
-        <v>5651.4033564814818</v>
+        <v>1130.2806712962963</v>
       </c>
       <c r="D11" s="18">
         <f t="shared" si="8"/>
@@ -55376,11 +55430,11 @@
       </c>
       <c r="M11" s="16">
         <f t="shared" si="2"/>
-        <v>117187500</v>
+        <v>23437500</v>
       </c>
       <c r="N11" s="16">
         <f t="shared" si="3"/>
-        <v>46875000</v>
+        <v>9375000</v>
       </c>
       <c r="Q11">
         <f t="shared" si="7"/>
@@ -55394,11 +55448,11 @@
       </c>
       <c r="B12" s="16">
         <f t="shared" si="0"/>
-        <v>195312500</v>
+        <v>39062500</v>
       </c>
       <c r="C12" s="16">
         <f t="shared" si="5"/>
-        <v>18838.011188271605</v>
+        <v>3767.602237654321</v>
       </c>
       <c r="D12" s="14">
         <f t="shared" ref="D12:D17" si="9">D11*1.5</f>
@@ -55414,11 +55468,11 @@
       </c>
       <c r="M12" s="16">
         <f t="shared" si="2"/>
-        <v>585937500</v>
+        <v>117187500</v>
       </c>
       <c r="N12" s="16">
         <f t="shared" si="3"/>
-        <v>234375000</v>
+        <v>46875000</v>
       </c>
       <c r="Q12">
         <f t="shared" si="7"/>
@@ -55432,11 +55486,11 @@
       </c>
       <c r="B13" s="16">
         <f t="shared" si="0"/>
-        <v>976562500</v>
+        <v>195312500</v>
       </c>
       <c r="C13" s="16">
         <f t="shared" si="5"/>
-        <v>62793.370627572011</v>
+        <v>12558.674125514402</v>
       </c>
       <c r="D13" s="14">
         <f t="shared" si="9"/>
@@ -55452,11 +55506,11 @@
       </c>
       <c r="M13" s="16">
         <f t="shared" si="2"/>
-        <v>2929687500</v>
+        <v>585937500</v>
       </c>
       <c r="N13" s="16">
         <f t="shared" si="3"/>
-        <v>1171875000</v>
+        <v>234375000</v>
       </c>
       <c r="Q13">
         <f t="shared" si="7"/>
@@ -55470,11 +55524,11 @@
       </c>
       <c r="B14" s="16">
         <f t="shared" si="0"/>
-        <v>4882812500</v>
+        <v>976562500</v>
       </c>
       <c r="C14" s="16">
         <f t="shared" si="5"/>
-        <v>209311.23542524007</v>
+        <v>41862.247085048009</v>
       </c>
       <c r="D14" s="14">
         <f t="shared" si="9"/>
@@ -55490,11 +55544,11 @@
       </c>
       <c r="M14" s="16">
         <f t="shared" si="2"/>
-        <v>14648437500</v>
+        <v>2929687500</v>
       </c>
       <c r="N14" s="16">
         <f t="shared" si="3"/>
-        <v>5859375000</v>
+        <v>1171875000</v>
       </c>
       <c r="Q14">
         <f t="shared" si="7"/>
@@ -55508,11 +55562,11 @@
       </c>
       <c r="B15" s="16">
         <f t="shared" si="0"/>
-        <v>24414062500</v>
+        <v>4882812500</v>
       </c>
       <c r="C15" s="16">
         <f t="shared" si="5"/>
-        <v>697704.11808413349</v>
+        <v>139540.8236168267</v>
       </c>
       <c r="D15" s="14">
         <f t="shared" si="9"/>
@@ -55528,11 +55582,11 @@
       </c>
       <c r="M15" s="16">
         <f t="shared" si="2"/>
-        <v>73242187500</v>
+        <v>14648437500</v>
       </c>
       <c r="N15" s="16">
         <f t="shared" si="3"/>
-        <v>29296875000</v>
+        <v>5859375000</v>
       </c>
       <c r="Q15">
         <f t="shared" si="7"/>
@@ -55546,11 +55600,11 @@
       </c>
       <c r="B16" s="16">
         <f t="shared" si="0"/>
-        <v>122070312500</v>
+        <v>24414062500</v>
       </c>
       <c r="C16" s="16">
         <f t="shared" si="5"/>
-        <v>2325680.3936137781</v>
+        <v>465136.0787227556</v>
       </c>
       <c r="D16" s="14">
         <f t="shared" si="9"/>
@@ -55566,11 +55620,11 @@
       </c>
       <c r="M16" s="16">
         <f t="shared" si="2"/>
-        <v>366210937500</v>
+        <v>73242187500</v>
       </c>
       <c r="N16" s="16">
         <f t="shared" si="3"/>
-        <v>146484375000</v>
+        <v>29296875000</v>
       </c>
       <c r="Q16">
         <f t="shared" si="7"/>
@@ -55584,11 +55638,11 @@
       </c>
       <c r="B17" s="16">
         <f t="shared" si="0"/>
-        <v>610351562500</v>
+        <v>122070312500</v>
       </c>
       <c r="C17" s="16">
         <f t="shared" si="5"/>
-        <v>7752267.9787125932</v>
+        <v>1550453.5957425185</v>
       </c>
       <c r="D17" s="14">
         <f t="shared" si="9"/>
@@ -55604,11 +55658,11 @@
       </c>
       <c r="M17" s="16">
         <f t="shared" si="2"/>
-        <v>1831054687500</v>
+        <v>366210937500</v>
       </c>
       <c r="N17" s="16">
         <f t="shared" si="3"/>
-        <v>732421875000</v>
+        <v>146484375000</v>
       </c>
       <c r="Q17">
         <f t="shared" si="7"/>
@@ -55622,11 +55676,11 @@
       </c>
       <c r="B18" s="16">
         <f t="shared" si="0"/>
-        <v>3051757812500</v>
+        <v>610351562500</v>
       </c>
       <c r="C18" s="16">
         <f t="shared" si="5"/>
-        <v>35237581.721420877</v>
+        <v>7047516.344284175</v>
       </c>
       <c r="D18">
         <f t="shared" ref="D18:D56" si="10">D17*1.1</f>
@@ -55642,11 +55696,11 @@
       </c>
       <c r="M18" s="16">
         <f t="shared" si="2"/>
-        <v>9155273437500</v>
+        <v>1831054687500</v>
       </c>
       <c r="N18" s="16">
         <f t="shared" si="3"/>
-        <v>3662109375000</v>
+        <v>732421875000</v>
       </c>
       <c r="Q18">
         <f t="shared" si="7"/>
@@ -55660,11 +55714,11 @@
       </c>
       <c r="B19" s="16">
         <f t="shared" si="0"/>
-        <v>15258789062500</v>
+        <v>3051757812500</v>
       </c>
       <c r="C19" s="16">
         <f t="shared" si="5"/>
-        <v>160170826.00645852</v>
+        <v>32034165.201291703</v>
       </c>
       <c r="D19">
         <f t="shared" si="10"/>
@@ -55680,11 +55734,11 @@
       </c>
       <c r="M19" s="16">
         <f t="shared" si="2"/>
-        <v>45776367187500</v>
+        <v>9155273437500</v>
       </c>
       <c r="N19" s="16">
         <f t="shared" si="3"/>
-        <v>18310546875000</v>
+        <v>3662109375000</v>
       </c>
       <c r="Q19">
         <f t="shared" si="7"/>
@@ -55698,11 +55752,11 @@
       </c>
       <c r="B20" s="16">
         <f t="shared" si="0"/>
-        <v>76293945312500</v>
+        <v>15258789062500</v>
       </c>
       <c r="C20" s="16">
         <f t="shared" si="5"/>
-        <v>728049209.12026584</v>
+        <v>145609841.82405317</v>
       </c>
       <c r="D20">
         <f t="shared" si="10"/>
@@ -55718,11 +55772,11 @@
       </c>
       <c r="M20" s="16">
         <f t="shared" si="2"/>
-        <v>228881835937500</v>
+        <v>45776367187500</v>
       </c>
       <c r="N20" s="16">
         <f t="shared" si="3"/>
-        <v>91552734375000</v>
+        <v>18310546875000</v>
       </c>
       <c r="Q20">
         <f t="shared" si="7"/>
@@ -55736,11 +55790,11 @@
       </c>
       <c r="B21" s="16">
         <f t="shared" si="0"/>
-        <v>381469726562500</v>
+        <v>76293945312500</v>
       </c>
       <c r="C21" s="16">
         <f t="shared" si="5"/>
-        <v>3309314586.9102988</v>
+        <v>661862917.38205981</v>
       </c>
       <c r="D21">
         <f t="shared" si="10"/>
@@ -55756,11 +55810,11 @@
       </c>
       <c r="M21" s="16">
         <f t="shared" si="2"/>
-        <v>1144409179687500</v>
+        <v>228881835937500</v>
       </c>
       <c r="N21" s="16">
         <f t="shared" si="3"/>
-        <v>457763671875000</v>
+        <v>91552734375000</v>
       </c>
       <c r="Q21">
         <f t="shared" si="7"/>
@@ -55774,11 +55828,11 @@
       </c>
       <c r="B22" s="16">
         <f t="shared" si="0"/>
-        <v>1907348632812500</v>
+        <v>381469726562500</v>
       </c>
       <c r="C22" s="16">
         <f t="shared" si="5"/>
-        <v>15042339031.410448</v>
+        <v>3008467806.2820897</v>
       </c>
       <c r="D22">
         <f t="shared" si="10"/>
@@ -55794,11 +55848,11 @@
       </c>
       <c r="M22" s="16">
         <f t="shared" si="2"/>
-        <v>5722045898437500</v>
+        <v>1144409179687500</v>
       </c>
       <c r="N22" s="16">
         <f t="shared" si="3"/>
-        <v>2288818359375000</v>
+        <v>457763671875000</v>
       </c>
       <c r="Q22">
         <f t="shared" si="7"/>
@@ -55812,11 +55866,11 @@
       </c>
       <c r="B23" s="16">
         <f t="shared" si="0"/>
-        <v>9536743164062500</v>
+        <v>1907348632812500</v>
       </c>
       <c r="C23" s="16">
         <f t="shared" si="5"/>
-        <v>68374268324.592941</v>
+        <v>13674853664.918589</v>
       </c>
       <c r="D23">
         <f t="shared" si="10"/>
@@ -55832,11 +55886,11 @@
       </c>
       <c r="M23" s="16">
         <f t="shared" si="2"/>
-        <v>2.86102294921875E+16</v>
+        <v>5722045898437500</v>
       </c>
       <c r="N23" s="16">
         <f t="shared" si="3"/>
-        <v>1.1444091796875E+16</v>
+        <v>2288818359375000</v>
       </c>
       <c r="Q23">
         <f t="shared" si="7"/>
@@ -55850,11 +55904,11 @@
       </c>
       <c r="B24" s="16">
         <f t="shared" si="0"/>
-        <v>4.7683715820312496E+16</v>
+        <v>9536743164062500</v>
       </c>
       <c r="C24" s="16">
         <f t="shared" si="5"/>
-        <v>310792128748.14966</v>
+        <v>62158425749.629944</v>
       </c>
       <c r="D24">
         <f t="shared" si="10"/>
@@ -55870,11 +55924,11 @@
       </c>
       <c r="M24" s="16">
         <f t="shared" si="2"/>
-        <v>1.4305114746093749E+17</v>
+        <v>2.86102294921875E+16</v>
       </c>
       <c r="N24" s="16">
         <f t="shared" si="3"/>
-        <v>5.7220458984374992E+16</v>
+        <v>1.1444091796875E+16</v>
       </c>
       <c r="Q24">
         <f t="shared" si="7"/>
@@ -55888,11 +55942,11 @@
       </c>
       <c r="B25" s="16">
         <f t="shared" si="0"/>
-        <v>2.384185791015625E+17</v>
+        <v>4.7683715820312496E+16</v>
       </c>
       <c r="C25" s="16">
         <f t="shared" si="5"/>
-        <v>1412691494309.7712</v>
+        <v>282538298861.95422</v>
       </c>
       <c r="D25">
         <f t="shared" si="10"/>
@@ -55908,11 +55962,11 @@
       </c>
       <c r="M25" s="16">
         <f t="shared" si="2"/>
-        <v>7.1525573730468749E+17</v>
+        <v>1.4305114746093749E+17</v>
       </c>
       <c r="N25" s="16">
         <f t="shared" si="3"/>
-        <v>2.8610229492187498E+17</v>
+        <v>5.7220458984374992E+16</v>
       </c>
       <c r="Q25">
         <f t="shared" si="7"/>
@@ -55926,11 +55980,11 @@
       </c>
       <c r="B26" s="16">
         <f t="shared" si="0"/>
-        <v>1.1920928955078124E+18</v>
+        <v>2.384185791015625E+17</v>
       </c>
       <c r="C26" s="16">
         <f t="shared" si="5"/>
-        <v>6421324974135.3232</v>
+        <v>1284264994827.0647</v>
       </c>
       <c r="D26">
         <f t="shared" si="10"/>
@@ -55946,11 +56000,11 @@
       </c>
       <c r="M26" s="16">
         <f t="shared" si="2"/>
-        <v>3.5762786865234371E+18</v>
+        <v>7.1525573730468749E+17</v>
       </c>
       <c r="N26" s="16">
         <f t="shared" si="3"/>
-        <v>1.4305114746093747E+18</v>
+        <v>2.8610229492187498E+17</v>
       </c>
       <c r="Q26">
         <f t="shared" si="7"/>
@@ -55964,11 +56018,11 @@
       </c>
       <c r="B27" s="16">
         <f t="shared" si="0"/>
-        <v>5.9604644775390618E+18</v>
+        <v>1.1920928955078124E+18</v>
       </c>
       <c r="C27" s="16">
         <f t="shared" si="5"/>
-        <v>29187840791524.191</v>
+        <v>5837568158304.8389</v>
       </c>
       <c r="D27">
         <f t="shared" si="10"/>
@@ -55984,11 +56038,11 @@
       </c>
       <c r="M27" s="16">
         <f t="shared" si="2"/>
-        <v>1.7881393432617185E+19</v>
+        <v>3.5762786865234371E+18</v>
       </c>
       <c r="N27" s="16">
         <f t="shared" si="3"/>
-        <v>7.1525573730468741E+18</v>
+        <v>1.4305114746093747E+18</v>
       </c>
       <c r="Q27">
         <f t="shared" si="7"/>
@@ -56002,11 +56056,11 @@
       </c>
       <c r="B28" s="16">
         <f t="shared" si="0"/>
-        <v>2.9802322387695309E+19</v>
+        <v>5.9604644775390618E+18</v>
       </c>
       <c r="C28" s="16">
         <f t="shared" si="5"/>
-        <v>132672003597837.23</v>
+        <v>26534400719567.445</v>
       </c>
       <c r="D28">
         <f t="shared" si="10"/>
@@ -56022,11 +56076,11 @@
       </c>
       <c r="M28" s="16">
         <f t="shared" si="2"/>
-        <v>8.940696716308593E+19</v>
+        <v>1.7881393432617185E+19</v>
       </c>
       <c r="N28" s="16">
         <f t="shared" si="3"/>
-        <v>3.5762786865234371E+19</v>
+        <v>7.1525573730468741E+18</v>
       </c>
       <c r="Q28">
         <f t="shared" si="7"/>
@@ -56040,11 +56094,11 @@
       </c>
       <c r="B29" s="16">
         <f t="shared" si="0"/>
-        <v>1.4901161193847656E+20</v>
+        <v>2.9802322387695309E+19</v>
       </c>
       <c r="C29" s="16">
         <f t="shared" si="5"/>
-        <v>603054561808351</v>
+        <v>120610912361670.19</v>
       </c>
       <c r="D29">
         <f t="shared" si="10"/>
@@ -56060,11 +56114,11 @@
       </c>
       <c r="M29" s="16">
         <f t="shared" si="2"/>
-        <v>4.470348358154297E+20</v>
+        <v>8.940696716308593E+19</v>
       </c>
       <c r="N29" s="16">
         <f t="shared" si="3"/>
-        <v>1.7881393432617186E+20</v>
+        <v>3.5762786865234371E+19</v>
       </c>
       <c r="Q29">
         <f t="shared" si="7"/>
@@ -56078,11 +56132,11 @@
       </c>
       <c r="B30" s="16">
         <f t="shared" si="0"/>
-        <v>7.4505805969238275E+20</v>
+        <v>1.4901161193847656E+20</v>
       </c>
       <c r="C30" s="16">
         <f t="shared" si="5"/>
-        <v>2741157099128867.5</v>
+        <v>548231419825773.5</v>
       </c>
       <c r="D30">
         <f t="shared" si="10"/>
@@ -56098,11 +56152,11 @@
       </c>
       <c r="M30" s="16">
         <f t="shared" si="2"/>
-        <v>2.2351741790771484E+21</v>
+        <v>4.470348358154297E+20</v>
       </c>
       <c r="N30" s="16">
         <f t="shared" si="3"/>
-        <v>8.9406967163085927E+20</v>
+        <v>1.7881393432617186E+20</v>
       </c>
       <c r="Q30">
         <f t="shared" si="7"/>
@@ -56116,11 +56170,11 @@
       </c>
       <c r="B31" s="16">
         <f t="shared" si="0"/>
-        <v>3.7252902984619136E+21</v>
+        <v>7.4505805969238275E+20</v>
       </c>
       <c r="C31" s="16">
         <f t="shared" si="5"/>
-        <v>1.2459804996040306E+16</v>
+        <v>2491960999208061.5</v>
       </c>
       <c r="D31">
         <f t="shared" si="10"/>
@@ -56136,11 +56190,11 @@
       </c>
       <c r="M31" s="16">
         <f t="shared" si="2"/>
-        <v>1.1175870895385741E+22</v>
+        <v>2.2351741790771484E+21</v>
       </c>
       <c r="N31" s="16">
         <f t="shared" si="3"/>
-        <v>4.4703483581542962E+21</v>
+        <v>8.9406967163085927E+20</v>
       </c>
       <c r="Q31">
         <f t="shared" si="7"/>
@@ -56154,11 +56208,11 @@
       </c>
       <c r="B32" s="16">
         <f t="shared" si="0"/>
-        <v>1.8626451492309568E+22</v>
+        <v>3.7252902984619136E+21</v>
       </c>
       <c r="C32" s="16">
         <f t="shared" si="5"/>
-        <v>5.6635477254728656E+16</v>
+        <v>1.1327095450945732E+16</v>
       </c>
       <c r="D32">
         <f t="shared" si="10"/>
@@ -56174,11 +56228,11 @@
       </c>
       <c r="M32" s="16">
         <f t="shared" si="2"/>
-        <v>5.5879354476928701E+22</v>
+        <v>1.1175870895385741E+22</v>
       </c>
       <c r="N32" s="16">
         <f t="shared" si="3"/>
-        <v>2.2351741790771479E+22</v>
+        <v>4.4703483581542962E+21</v>
       </c>
       <c r="Q32">
         <f t="shared" si="7"/>
@@ -56192,11 +56246,11 @@
       </c>
       <c r="B33" s="16">
         <f t="shared" si="0"/>
-        <v>9.313225746154784E+22</v>
+        <v>1.8626451492309568E+22</v>
       </c>
       <c r="C33" s="16">
         <f t="shared" si="5"/>
-        <v>2.5743398752149392E+17</v>
+        <v>5.1486797504298784E+16</v>
       </c>
       <c r="D33">
         <f t="shared" si="10"/>
@@ -56212,11 +56266,11 @@
       </c>
       <c r="M33" s="16">
         <f t="shared" si="2"/>
-        <v>2.7939677238464352E+23</v>
+        <v>5.5879354476928701E+22</v>
       </c>
       <c r="N33" s="16">
         <f t="shared" si="3"/>
-        <v>1.117587089538574E+23</v>
+        <v>2.2351741790771479E+22</v>
       </c>
       <c r="Q33">
         <f t="shared" si="7"/>
@@ -56230,11 +56284,11 @@
       </c>
       <c r="B34" s="16">
         <f t="shared" si="0"/>
-        <v>4.6566128730773923E+23</v>
+        <v>9.313225746154784E+22</v>
       </c>
       <c r="C34" s="16">
         <f t="shared" si="5"/>
-        <v>1.1701544887340631E+18</v>
+        <v>2.3403089774681258E+17</v>
       </c>
       <c r="D34">
         <f t="shared" si="10"/>
@@ -56250,11 +56304,11 @@
       </c>
       <c r="M34" s="16">
         <f t="shared" si="2"/>
-        <v>1.3969838619232177E+24</v>
+        <v>2.7939677238464352E+23</v>
       </c>
       <c r="N34" s="16">
         <f t="shared" si="3"/>
-        <v>5.5879354476928704E+23</v>
+        <v>1.117587089538574E+23</v>
       </c>
       <c r="Q34">
         <f t="shared" si="7"/>
@@ -56268,11 +56322,11 @@
       </c>
       <c r="B35" s="16">
         <f t="shared" si="0"/>
-        <v>2.3283064365386962E+24</v>
+        <v>4.6566128730773923E+23</v>
       </c>
       <c r="C35" s="16">
         <f t="shared" si="5"/>
-        <v>5.3188840397002865E+18</v>
+        <v>1.0637768079400573E+18</v>
       </c>
       <c r="D35">
         <f t="shared" si="10"/>
@@ -56288,11 +56342,11 @@
       </c>
       <c r="M35" s="16">
         <f t="shared" si="2"/>
-        <v>6.9849193096160882E+24</v>
+        <v>1.3969838619232177E+24</v>
       </c>
       <c r="N35" s="16">
         <f t="shared" si="3"/>
-        <v>2.7939677238464354E+24</v>
+        <v>5.5879354476928704E+23</v>
       </c>
       <c r="Q35">
         <f t="shared" si="7"/>
@@ -56306,11 +56360,11 @@
       </c>
       <c r="B36" s="16">
         <f t="shared" ref="B36:B67" si="11">B35*I$3</f>
-        <v>1.1641532182693481E+25</v>
+        <v>2.3283064365386962E+24</v>
       </c>
       <c r="C36" s="16">
         <f t="shared" si="5"/>
-        <v>2.4176745635001299E+19</v>
+        <v>4.8353491270002596E+18</v>
       </c>
       <c r="D36">
         <f t="shared" si="10"/>
@@ -56326,11 +56380,11 @@
       </c>
       <c r="M36" s="16">
         <f t="shared" si="2"/>
-        <v>3.4924596548080443E+25</v>
+        <v>6.9849193096160882E+24</v>
       </c>
       <c r="N36" s="16">
         <f t="shared" si="3"/>
-        <v>1.3969838619232176E+25</v>
+        <v>2.7939677238464354E+24</v>
       </c>
       <c r="Q36">
         <f t="shared" si="7"/>
@@ -56344,11 +56398,11 @@
       </c>
       <c r="B37" s="16">
         <f t="shared" si="11"/>
-        <v>5.8207660913467401E+25</v>
+        <v>1.1641532182693481E+25</v>
       </c>
       <c r="C37" s="16">
         <f t="shared" si="5"/>
-        <v>1.0989429834091499E+20</v>
+        <v>2.1978859668182999E+19</v>
       </c>
       <c r="D37">
         <f t="shared" si="10"/>
@@ -56364,11 +56418,11 @@
       </c>
       <c r="M37" s="16">
         <f t="shared" si="2"/>
-        <v>1.7462298274040222E+26</v>
+        <v>3.4924596548080443E+25</v>
       </c>
       <c r="N37" s="16">
         <f t="shared" si="3"/>
-        <v>6.9849193096160878E+25</v>
+        <v>1.3969838619232176E+25</v>
       </c>
       <c r="Q37">
         <f t="shared" si="7"/>
@@ -56382,11 +56436,11 @@
       </c>
       <c r="B38" s="16">
         <f t="shared" si="11"/>
-        <v>2.9103830456733699E+26</v>
+        <v>5.8207660913467401E+25</v>
       </c>
       <c r="C38" s="16">
         <f t="shared" si="5"/>
-        <v>4.9951953791324973E+20</v>
+        <v>9.9903907582649958E+19</v>
       </c>
       <c r="D38">
         <f t="shared" si="10"/>
@@ -56402,11 +56456,11 @@
       </c>
       <c r="M38" s="16">
         <f t="shared" si="2"/>
-        <v>8.7311491370201103E+26</v>
+        <v>1.7462298274040222E+26</v>
       </c>
       <c r="N38" s="16">
         <f t="shared" si="3"/>
-        <v>3.4924596548080437E+26</v>
+        <v>6.9849193096160878E+25</v>
       </c>
       <c r="Q38">
         <f t="shared" si="7"/>
@@ -56420,11 +56474,11 @@
       </c>
       <c r="B39" s="16">
         <f t="shared" si="11"/>
-        <v>1.4551915228366849E+27</v>
+        <v>2.9103830456733699E+26</v>
       </c>
       <c r="C39" s="16">
         <f t="shared" si="5"/>
-        <v>2.2705433541511353E+21</v>
+        <v>4.541086708302271E+20</v>
       </c>
       <c r="D39">
         <f t="shared" si="10"/>
@@ -56440,11 +56494,11 @@
       </c>
       <c r="M39" s="16">
         <f t="shared" si="2"/>
-        <v>4.3655745685100546E+27</v>
+        <v>8.7311491370201103E+26</v>
       </c>
       <c r="N39" s="16">
         <f t="shared" si="3"/>
-        <v>1.7462298274040218E+27</v>
+        <v>3.4924596548080437E+26</v>
       </c>
       <c r="Q39">
         <f t="shared" si="7"/>
@@ -56458,11 +56512,11 @@
       </c>
       <c r="B40" s="16">
         <f t="shared" si="11"/>
-        <v>7.2759576141834244E+27</v>
+        <v>1.4551915228366849E+27</v>
       </c>
       <c r="C40" s="16">
         <f t="shared" si="5"/>
-        <v>1.0320651609777885E+22</v>
+        <v>2.0641303219555771E+21</v>
       </c>
       <c r="D40">
         <f t="shared" si="10"/>
@@ -56478,11 +56532,11 @@
       </c>
       <c r="M40" s="16">
         <f t="shared" si="2"/>
-        <v>2.1827872842550273E+28</v>
+        <v>4.3655745685100546E+27</v>
       </c>
       <c r="N40" s="16">
         <f t="shared" si="3"/>
-        <v>8.7311491370201092E+27</v>
+        <v>1.7462298274040218E+27</v>
       </c>
       <c r="Q40">
         <f t="shared" si="7"/>
@@ -56496,11 +56550,11 @@
       </c>
       <c r="B41" s="16">
         <f t="shared" si="11"/>
-        <v>3.6379788070917122E+28</v>
+        <v>7.2759576141834244E+27</v>
       </c>
       <c r="C41" s="16">
         <f t="shared" si="5"/>
-        <v>4.6912052771717655E+22</v>
+        <v>9.382410554343532E+21</v>
       </c>
       <c r="D41">
         <f t="shared" si="10"/>
@@ -56516,11 +56570,11 @@
       </c>
       <c r="M41" s="16">
         <f t="shared" si="2"/>
-        <v>1.0913936421275136E+29</v>
+        <v>2.1827872842550273E+28</v>
       </c>
       <c r="N41" s="16">
         <f t="shared" si="3"/>
-        <v>4.3655745685100546E+28</v>
+        <v>8.7311491370201092E+27</v>
       </c>
       <c r="Q41">
         <f t="shared" si="7"/>
@@ -56534,11 +56588,11 @@
       </c>
       <c r="B42" s="16">
         <f t="shared" si="11"/>
-        <v>1.8189894035458561E+29</v>
+        <v>3.6379788070917122E+28</v>
       </c>
       <c r="C42" s="16">
         <f t="shared" si="5"/>
-        <v>2.1323660350780752E+23</v>
+        <v>4.2647320701561507E+22</v>
       </c>
       <c r="D42">
         <f t="shared" si="10"/>
@@ -56554,11 +56608,11 @@
       </c>
       <c r="M42" s="16">
         <f t="shared" si="2"/>
-        <v>5.4569682106375684E+29</v>
+        <v>1.0913936421275136E+29</v>
       </c>
       <c r="N42" s="16">
         <f t="shared" si="3"/>
-        <v>2.1827872842550272E+29</v>
+        <v>4.3655745685100546E+28</v>
       </c>
       <c r="Q42">
         <f t="shared" si="7"/>
@@ -56572,11 +56626,11 @@
       </c>
       <c r="B43" s="16">
         <f t="shared" si="11"/>
-        <v>9.0949470177292814E+29</v>
+        <v>1.8189894035458561E+29</v>
       </c>
       <c r="C43" s="16">
         <f t="shared" si="5"/>
-        <v>9.692572886718525E+23</v>
+        <v>1.9385145773437048E+23</v>
       </c>
       <c r="D43">
         <f t="shared" si="10"/>
@@ -56592,11 +56646,11 @@
       </c>
       <c r="M43" s="16">
         <f t="shared" si="2"/>
-        <v>2.7284841053187844E+30</v>
+        <v>5.4569682106375684E+29</v>
       </c>
       <c r="N43" s="16">
         <f t="shared" si="3"/>
-        <v>1.0913936421275137E+30</v>
+        <v>2.1827872842550272E+29</v>
       </c>
       <c r="Q43">
         <f t="shared" si="7"/>
@@ -56610,11 +56664,11 @@
       </c>
       <c r="B44" s="16">
         <f t="shared" si="11"/>
-        <v>4.5474735088646407E+30</v>
+        <v>9.0949470177292814E+29</v>
       </c>
       <c r="C44" s="16">
         <f t="shared" si="5"/>
-        <v>4.4057149485084199E+24</v>
+        <v>8.8114298970168396E+23</v>
       </c>
       <c r="D44">
         <f t="shared" si="10"/>
@@ -56630,11 +56684,11 @@
       </c>
       <c r="M44" s="16">
         <f t="shared" si="2"/>
-        <v>1.3642420526593922E+31</v>
+        <v>2.7284841053187844E+30</v>
       </c>
       <c r="N44" s="16">
         <f t="shared" si="3"/>
-        <v>5.4569682106375688E+30</v>
+        <v>1.0913936421275137E+30</v>
       </c>
       <c r="Q44">
         <f t="shared" si="7"/>
@@ -56648,11 +56702,11 @@
       </c>
       <c r="B45" s="16">
         <f t="shared" si="11"/>
-        <v>2.2737367544323203E+31</v>
+        <v>4.5474735088646407E+30</v>
       </c>
       <c r="C45" s="16">
         <f t="shared" si="5"/>
-        <v>2.0025977038674634E+25</v>
+        <v>4.0051954077349265E+24</v>
       </c>
       <c r="D45">
         <f t="shared" si="10"/>
@@ -56668,11 +56722,11 @@
       </c>
       <c r="M45" s="16">
         <f t="shared" si="2"/>
-        <v>6.8212102632969606E+31</v>
+        <v>1.3642420526593922E+31</v>
       </c>
       <c r="N45" s="16">
         <f t="shared" si="3"/>
-        <v>2.7284841053187844E+31</v>
+        <v>5.4569682106375688E+30</v>
       </c>
       <c r="Q45">
         <f t="shared" si="7"/>
@@ -56686,11 +56740,11 @@
       </c>
       <c r="B46" s="16">
         <f t="shared" si="11"/>
-        <v>1.1368683772161602E+32</v>
+        <v>2.2737367544323203E+31</v>
       </c>
       <c r="C46" s="16">
         <f t="shared" si="5"/>
-        <v>9.1027168357611963E+25</v>
+        <v>1.820543367152239E+25</v>
       </c>
       <c r="D46">
         <f t="shared" si="10"/>
@@ -56706,11 +56760,11 @@
       </c>
       <c r="M46" s="16">
         <f t="shared" si="2"/>
-        <v>3.4106051316484803E+32</v>
+        <v>6.8212102632969606E+31</v>
       </c>
       <c r="N46" s="16">
         <f t="shared" si="3"/>
-        <v>1.3642420526593923E+32</v>
+        <v>2.7284841053187844E+31</v>
       </c>
       <c r="Q46">
         <f t="shared" si="7"/>
@@ -56724,11 +56778,11 @@
       </c>
       <c r="B47" s="16">
         <f t="shared" si="11"/>
-        <v>5.6843418860808014E+32</v>
+        <v>1.1368683772161602E+32</v>
       </c>
       <c r="C47" s="16">
         <f t="shared" si="5"/>
-        <v>4.1375985617096349E+26</v>
+        <v>8.2751971234192689E+25</v>
       </c>
       <c r="D47">
         <f t="shared" si="10"/>
@@ -56744,11 +56798,11 @@
       </c>
       <c r="M47" s="16">
         <f t="shared" si="2"/>
-        <v>1.7053025658242403E+33</v>
+        <v>3.4106051316484803E+32</v>
       </c>
       <c r="N47" s="16">
         <f t="shared" si="3"/>
-        <v>6.821210263296962E+32</v>
+        <v>1.3642420526593923E+32</v>
       </c>
       <c r="Q47">
         <f t="shared" si="7"/>
@@ -56762,11 +56816,11 @@
       </c>
       <c r="B48" s="16">
         <f t="shared" si="11"/>
-        <v>2.8421709430404009E+33</v>
+        <v>5.6843418860808014E+32</v>
       </c>
       <c r="C48" s="16">
         <f t="shared" si="5"/>
-        <v>1.8807266189589246E+27</v>
+        <v>3.761453237917849E+26</v>
       </c>
       <c r="D48">
         <f t="shared" si="10"/>
@@ -56782,11 +56836,11 @@
       </c>
       <c r="M48" s="16">
         <f t="shared" si="2"/>
-        <v>8.5265128291212026E+33</v>
+        <v>1.7053025658242403E+33</v>
       </c>
       <c r="N48" s="16">
         <f t="shared" si="3"/>
-        <v>3.4106051316484812E+33</v>
+        <v>6.821210263296962E+32</v>
       </c>
       <c r="Q48">
         <f t="shared" si="7"/>
@@ -56800,11 +56854,11 @@
       </c>
       <c r="B49" s="16">
         <f t="shared" si="11"/>
-        <v>1.4210854715202004E+34</v>
+        <v>2.8421709430404009E+33</v>
       </c>
       <c r="C49" s="16">
         <f t="shared" si="5"/>
-        <v>8.5487573589042022E+27</v>
+        <v>1.7097514717808403E+27</v>
       </c>
       <c r="D49">
         <f t="shared" si="10"/>
@@ -56820,11 +56874,11 @@
       </c>
       <c r="M49" s="16">
         <f t="shared" si="2"/>
-        <v>4.2632564145606011E+34</v>
+        <v>8.5265128291212026E+33</v>
       </c>
       <c r="N49" s="16">
         <f t="shared" si="3"/>
-        <v>1.7053025658242405E+34</v>
+        <v>3.4106051316484812E+33</v>
       </c>
       <c r="Q49">
         <f t="shared" si="7"/>
@@ -56838,11 +56892,11 @@
       </c>
       <c r="B50" s="16">
         <f t="shared" si="11"/>
-        <v>7.1054273576010024E+34</v>
+        <v>1.4210854715202004E+34</v>
       </c>
       <c r="C50" s="16">
         <f t="shared" si="5"/>
-        <v>3.8857987995019098E+28</v>
+        <v>7.7715975990038196E+27</v>
       </c>
       <c r="D50">
         <f t="shared" si="10"/>
@@ -56858,11 +56912,11 @@
       </c>
       <c r="M50" s="16">
         <f t="shared" si="2"/>
-        <v>2.1316282072803007E+35</v>
+        <v>4.2632564145606011E+34</v>
       </c>
       <c r="N50" s="16">
         <f t="shared" si="3"/>
-        <v>8.5265128291212021E+34</v>
+        <v>1.7053025658242405E+34</v>
       </c>
       <c r="Q50">
         <f t="shared" si="7"/>
@@ -56876,11 +56930,11 @@
       </c>
       <c r="B51" s="16">
         <f t="shared" si="11"/>
-        <v>3.5527136788005012E+35</v>
+        <v>7.1054273576010024E+34</v>
       </c>
       <c r="C51" s="16">
         <f t="shared" si="5"/>
-        <v>1.7662721815917771E+29</v>
+        <v>3.5325443631835541E+28</v>
       </c>
       <c r="D51">
         <f t="shared" si="10"/>
@@ -56896,11 +56950,11 @@
       </c>
       <c r="M51" s="16">
         <f t="shared" si="2"/>
-        <v>1.0658141036401504E+36</v>
+        <v>2.1316282072803007E+35</v>
       </c>
       <c r="N51" s="16">
         <f t="shared" si="3"/>
-        <v>4.2632564145606014E+35</v>
+        <v>8.5265128291212021E+34</v>
       </c>
       <c r="Q51">
         <f t="shared" si="7"/>
@@ -56914,11 +56968,11 @@
       </c>
       <c r="B52" s="16">
         <f t="shared" si="11"/>
-        <v>1.7763568394002505E+36</v>
+        <v>3.5527136788005012E+35</v>
       </c>
       <c r="C52" s="16">
         <f t="shared" si="5"/>
-        <v>8.028509916326256E+29</v>
+        <v>1.6057019832652513E+29</v>
       </c>
       <c r="D52">
         <f t="shared" si="10"/>
@@ -56934,11 +56988,11 @@
       </c>
       <c r="M52" s="16">
         <f t="shared" si="2"/>
-        <v>5.3290705182007514E+36</v>
+        <v>1.0658141036401504E+36</v>
       </c>
       <c r="N52" s="16">
         <f t="shared" si="3"/>
-        <v>2.1316282072803004E+36</v>
+        <v>4.2632564145606014E+35</v>
       </c>
       <c r="Q52">
         <f t="shared" si="7"/>
@@ -56952,11 +57006,11 @@
       </c>
       <c r="B53" s="16">
         <f t="shared" si="11"/>
-        <v>8.8817841970012523E+36</v>
+        <v>1.7763568394002505E+36</v>
       </c>
       <c r="C53" s="16">
         <f t="shared" si="5"/>
-        <v>3.6493226892392075E+30</v>
+        <v>7.2986453784784152E+29</v>
       </c>
       <c r="D53">
         <f t="shared" si="10"/>
@@ -56972,11 +57026,11 @@
       </c>
       <c r="M53" s="16">
         <f t="shared" si="2"/>
-        <v>2.6645352591003757E+37</v>
+        <v>5.3290705182007514E+36</v>
       </c>
       <c r="N53" s="16">
         <f t="shared" si="3"/>
-        <v>1.0658141036401503E+37</v>
+        <v>2.1316282072803004E+36</v>
       </c>
       <c r="Q53">
         <f t="shared" si="7"/>
@@ -56990,11 +57044,11 @@
       </c>
       <c r="B54" s="16">
         <f t="shared" si="11"/>
-        <v>4.4408920985006261E+37</v>
+        <v>8.8817841970012523E+36</v>
       </c>
       <c r="C54" s="16">
         <f t="shared" si="5"/>
-        <v>1.658783040563276E+31</v>
+        <v>3.3175660811265521E+30</v>
       </c>
       <c r="D54">
         <f t="shared" si="10"/>
@@ -57010,11 +57064,11 @@
       </c>
       <c r="M54" s="16">
         <f t="shared" si="2"/>
-        <v>1.3322676295501878E+38</v>
+        <v>2.6645352591003757E+37</v>
       </c>
       <c r="N54" s="16">
         <f t="shared" si="3"/>
-        <v>5.3290705182007514E+37</v>
+        <v>1.0658141036401503E+37</v>
       </c>
       <c r="Q54">
         <f t="shared" si="7"/>
@@ -57028,11 +57082,11 @@
       </c>
       <c r="B55" s="16">
         <f t="shared" si="11"/>
-        <v>2.2204460492503133E+38</v>
+        <v>4.4408920985006261E+37</v>
       </c>
       <c r="C55" s="16">
         <f t="shared" si="5"/>
-        <v>7.5399229116512538E+31</v>
+        <v>1.5079845823302506E+31</v>
       </c>
       <c r="D55">
         <f t="shared" si="10"/>
@@ -57048,11 +57102,11 @@
       </c>
       <c r="M55" s="16">
         <f t="shared" si="2"/>
-        <v>6.6613381477509398E+38</v>
+        <v>1.3322676295501878E+38</v>
       </c>
       <c r="N55" s="16">
         <f t="shared" si="3"/>
-        <v>2.6645352591003757E+38</v>
+        <v>5.3290705182007514E+37</v>
       </c>
       <c r="Q55">
         <f t="shared" si="7"/>
@@ -57066,11 +57120,11 @@
       </c>
       <c r="B56" s="16">
         <f t="shared" si="11"/>
-        <v>1.1102230246251567E+39</v>
+        <v>2.2204460492503133E+38</v>
       </c>
       <c r="C56" s="16">
         <f t="shared" si="5"/>
-        <v>3.4272376871142063E+32</v>
+        <v>6.8544753742284126E+31</v>
       </c>
       <c r="D56">
         <f t="shared" si="10"/>
@@ -57086,11 +57140,11 @@
       </c>
       <c r="M56" s="16">
         <f t="shared" si="2"/>
-        <v>3.3306690738754704E+39</v>
+        <v>6.6613381477509398E+38</v>
       </c>
       <c r="N56" s="16">
         <f t="shared" si="3"/>
-        <v>1.332267629550188E+39</v>
+        <v>2.6645352591003757E+38</v>
       </c>
       <c r="Q56">
         <f t="shared" si="7"/>
@@ -57104,11 +57158,11 @@
       </c>
       <c r="B57" s="16">
         <f t="shared" si="11"/>
-        <v>5.5511151231257832E+39</v>
+        <v>1.1102230246251567E+39</v>
       </c>
       <c r="C57" s="16">
         <f t="shared" si="5"/>
-        <v>1.5578353123246389E+33</v>
+        <v>3.1156706246492782E+32</v>
       </c>
       <c r="D57">
         <f t="shared" ref="D57:D83" si="12">D56*1.1</f>
@@ -57124,11 +57178,11 @@
       </c>
       <c r="M57" s="16">
         <f t="shared" si="2"/>
-        <v>1.6653345369377351E+40</v>
+        <v>3.3306690738754704E+39</v>
       </c>
       <c r="N57" s="16">
         <f t="shared" si="3"/>
-        <v>6.6613381477509396E+39</v>
+        <v>1.332267629550188E+39</v>
       </c>
       <c r="Q57">
         <f t="shared" si="7"/>
@@ -57142,11 +57196,11 @@
       </c>
       <c r="B58" s="16">
         <f t="shared" si="11"/>
-        <v>2.7755575615628915E+40</v>
+        <v>5.5511151231257832E+39</v>
       </c>
       <c r="C58" s="16">
         <f t="shared" si="5"/>
-        <v>7.0810696014756317E+33</v>
+        <v>1.4162139202951264E+33</v>
       </c>
       <c r="D58">
         <f t="shared" si="12"/>
@@ -57162,11 +57216,11 @@
       </c>
       <c r="M58" s="16">
         <f t="shared" si="2"/>
-        <v>8.326672684688674E+40</v>
+        <v>1.6653345369377351E+40</v>
       </c>
       <c r="N58" s="16">
         <f t="shared" si="3"/>
-        <v>3.3306690738754697E+40</v>
+        <v>6.6613381477509396E+39</v>
       </c>
       <c r="Q58">
         <f t="shared" si="7"/>
@@ -57180,11 +57234,11 @@
       </c>
       <c r="B59" s="16">
         <f t="shared" si="11"/>
-        <v>1.3877787807814458E+41</v>
+        <v>2.7755575615628915E+40</v>
       </c>
       <c r="C59" s="16">
         <f t="shared" si="5"/>
-        <v>3.218668000670742E+34</v>
+        <v>6.4373360013414833E+33</v>
       </c>
       <c r="D59">
         <f t="shared" si="12"/>
@@ -57200,11 +57254,11 @@
       </c>
       <c r="M59" s="16">
         <f t="shared" si="2"/>
-        <v>4.1633363423443374E+41</v>
+        <v>8.326672684688674E+40</v>
       </c>
       <c r="N59" s="16">
         <f t="shared" si="3"/>
-        <v>1.6653345369377348E+41</v>
+        <v>3.3306690738754697E+40</v>
       </c>
       <c r="Q59">
         <f t="shared" si="7"/>
@@ -57218,11 +57272,11 @@
       </c>
       <c r="B60" s="16">
         <f t="shared" si="11"/>
-        <v>6.938893903907229E+41</v>
+        <v>1.3877787807814458E+41</v>
       </c>
       <c r="C60" s="16">
         <f t="shared" si="5"/>
-        <v>1.4630309093957914E+35</v>
+        <v>2.9260618187915828E+34</v>
       </c>
       <c r="D60">
         <f t="shared" si="12"/>
@@ -57238,11 +57292,11 @@
       </c>
       <c r="M60" s="16">
         <f t="shared" si="2"/>
-        <v>2.0816681711721685E+42</v>
+        <v>4.1633363423443374E+41</v>
       </c>
       <c r="N60" s="16">
         <f t="shared" si="3"/>
-        <v>8.3266726846886747E+41</v>
+        <v>1.6653345369377348E+41</v>
       </c>
       <c r="Q60">
         <f t="shared" si="7"/>
@@ -57256,11 +57310,11 @@
       </c>
       <c r="B61" s="16">
         <f t="shared" si="11"/>
-        <v>3.4694469519536146E+42</v>
+        <v>6.938893903907229E+41</v>
       </c>
       <c r="C61" s="16">
         <f t="shared" si="5"/>
-        <v>6.6501404972535968E+35</v>
+        <v>1.3300280994507195E+35</v>
       </c>
       <c r="D61">
         <f t="shared" si="12"/>
@@ -57276,11 +57330,11 @@
       </c>
       <c r="M61" s="16">
         <f t="shared" si="2"/>
-        <v>1.0408340855860845E+43</v>
+        <v>2.0816681711721685E+42</v>
       </c>
       <c r="N61" s="16">
         <f t="shared" si="3"/>
-        <v>4.1633363423443377E+42</v>
+        <v>8.3266726846886747E+41</v>
       </c>
       <c r="Q61">
         <f t="shared" si="7"/>
@@ -57294,11 +57348,11 @@
       </c>
       <c r="B62" s="16">
         <f t="shared" si="11"/>
-        <v>1.7347234759768073E+43</v>
+        <v>3.4694469519536146E+42</v>
       </c>
       <c r="C62" s="16">
         <f t="shared" si="5"/>
-        <v>3.022791135115271E+36</v>
+        <v>6.045582270230542E+35</v>
       </c>
       <c r="D62">
         <f t="shared" si="12"/>
@@ -57314,11 +57368,11 @@
       </c>
       <c r="M62" s="16">
         <f t="shared" si="2"/>
-        <v>5.2041704279304213E+43</v>
+        <v>1.0408340855860845E+43</v>
       </c>
       <c r="N62" s="16">
         <f t="shared" si="3"/>
-        <v>2.0816681711721687E+43</v>
+        <v>4.1633363423443377E+42</v>
       </c>
       <c r="Q62">
         <f t="shared" si="7"/>
@@ -57332,11 +57386,11 @@
       </c>
       <c r="B63" s="16">
         <f t="shared" si="11"/>
-        <v>8.6736173798840368E+43</v>
+        <v>1.7347234759768073E+43</v>
       </c>
       <c r="C63" s="16">
         <f t="shared" si="5"/>
-        <v>1.3739959705069413E+37</v>
+        <v>2.7479919410138821E+36</v>
       </c>
       <c r="D63">
         <f t="shared" si="12"/>
@@ -57352,11 +57406,11 @@
       </c>
       <c r="M63" s="16">
         <f t="shared" si="2"/>
-        <v>2.602085213965211E+44</v>
+        <v>5.2041704279304213E+43</v>
       </c>
       <c r="N63" s="16">
         <f t="shared" si="3"/>
-        <v>1.0408340855860845E+44</v>
+        <v>2.0816681711721687E+43</v>
       </c>
       <c r="Q63">
         <f t="shared" si="7"/>
@@ -57370,11 +57424,11 @@
       </c>
       <c r="B64" s="16">
         <f t="shared" si="11"/>
-        <v>4.3368086899420188E+44</v>
+        <v>8.6736173798840368E+43</v>
       </c>
       <c r="C64" s="16">
         <f t="shared" si="5"/>
-        <v>6.2454362295770054E+37</v>
+        <v>1.2490872459154011E+37</v>
       </c>
       <c r="D64">
         <f t="shared" si="12"/>
@@ -57390,11 +57444,11 @@
       </c>
       <c r="M64" s="16">
         <f t="shared" si="2"/>
-        <v>1.3010426069826056E+45</v>
+        <v>2.602085213965211E+44</v>
       </c>
       <c r="N64" s="16">
         <f t="shared" si="3"/>
-        <v>5.2041704279304221E+44</v>
+        <v>1.0408340855860845E+44</v>
       </c>
       <c r="Q64">
         <f t="shared" si="7"/>
@@ -57408,11 +57462,11 @@
       </c>
       <c r="B65" s="16">
         <f t="shared" si="11"/>
-        <v>2.1684043449710092E+45</v>
+        <v>4.3368086899420188E+44</v>
       </c>
       <c r="C65" s="16">
         <f t="shared" si="5"/>
-        <v>2.8388346498077295E+38</v>
+        <v>5.6776692996154592E+37</v>
       </c>
       <c r="D65">
         <f t="shared" si="12"/>
@@ -57428,11 +57482,11 @@
       </c>
       <c r="M65" s="16">
         <f t="shared" si="2"/>
-        <v>6.5052130349130271E+45</v>
+        <v>1.3010426069826056E+45</v>
       </c>
       <c r="N65" s="16">
         <f t="shared" si="3"/>
-        <v>2.602085213965211E+45</v>
+        <v>5.2041704279304221E+44</v>
       </c>
       <c r="Q65">
         <f t="shared" si="7"/>
@@ -57446,11 +57500,11 @@
       </c>
       <c r="B66" s="16">
         <f t="shared" si="11"/>
-        <v>1.0842021724855047E+46</v>
+        <v>2.1684043449710092E+45</v>
       </c>
       <c r="C66" s="16">
         <f t="shared" si="5"/>
-        <v>1.2903793862762406E+39</v>
+        <v>2.5807587725524809E+38</v>
       </c>
       <c r="D66">
         <f t="shared" si="12"/>
@@ -57466,11 +57520,11 @@
       </c>
       <c r="M66" s="16">
         <f t="shared" si="2"/>
-        <v>3.252606517456514E+46</v>
+        <v>6.5052130349130271E+45</v>
       </c>
       <c r="N66" s="16">
         <f t="shared" si="3"/>
-        <v>1.3010426069826057E+46</v>
+        <v>2.602085213965211E+45</v>
       </c>
       <c r="Q66">
         <f t="shared" si="7"/>
@@ -57484,11 +57538,11 @@
       </c>
       <c r="B67" s="16">
         <f t="shared" si="11"/>
-        <v>5.4210108624275229E+46</v>
+        <v>1.0842021724855047E+46</v>
       </c>
       <c r="C67" s="16">
         <f t="shared" si="5"/>
-        <v>5.8653608467101839E+39</v>
+        <v>1.1730721693420369E+39</v>
       </c>
       <c r="D67">
         <f t="shared" si="12"/>
@@ -57504,11 +57558,11 @@
       </c>
       <c r="M67" s="16">
         <f t="shared" si="2"/>
-        <v>1.6263032587282569E+47</v>
+        <v>3.252606517456514E+46</v>
       </c>
       <c r="N67" s="16">
         <f t="shared" si="3"/>
-        <v>6.5052130349130271E+46</v>
+        <v>1.3010426069826057E+46</v>
       </c>
       <c r="Q67">
         <f t="shared" si="7"/>
@@ -57522,11 +57576,11 @@
       </c>
       <c r="B68" s="16">
         <f t="shared" ref="B68:B83" si="14">B67*I$3</f>
-        <v>2.7105054312137614E+47</v>
+        <v>5.4210108624275229E+46</v>
       </c>
       <c r="C68" s="16">
         <f t="shared" si="5"/>
-        <v>2.6660731121409922E+40</v>
+        <v>5.3321462242819843E+39</v>
       </c>
       <c r="D68">
         <f t="shared" si="12"/>
@@ -57542,11 +57596,11 @@
       </c>
       <c r="M68" s="16">
         <f t="shared" ref="M68:M83" si="16">B68*I$5</f>
-        <v>8.1315162936412851E+47</v>
+        <v>1.6263032587282569E+47</v>
       </c>
       <c r="N68" s="16">
         <f t="shared" ref="N68:N83" si="17">B68*I$6</f>
-        <v>3.2526065174565137E+47</v>
+        <v>6.5052130349130271E+46</v>
       </c>
       <c r="Q68">
         <f t="shared" si="7"/>
@@ -57560,11 +57614,11 @@
       </c>
       <c r="B69" s="16">
         <f t="shared" si="14"/>
-        <v>1.3552527156068806E+48</v>
+        <v>2.7105054312137614E+47</v>
       </c>
       <c r="C69" s="16">
         <f t="shared" ref="C69:C83" si="19">B69/(D69*3600)</f>
-        <v>1.2118514146095416E+41</v>
+        <v>2.4237028292190834E+40</v>
       </c>
       <c r="D69">
         <f t="shared" si="12"/>
@@ -57580,11 +57634,11 @@
       </c>
       <c r="M69" s="16">
         <f t="shared" si="16"/>
-        <v>4.0657581468206419E+48</v>
+        <v>8.1315162936412851E+47</v>
       </c>
       <c r="N69" s="16">
         <f t="shared" si="17"/>
-        <v>1.6263032587282567E+48</v>
+        <v>3.2526065174565137E+47</v>
       </c>
       <c r="Q69">
         <f t="shared" ref="Q69:Q83" si="20">Q68*J$11</f>
@@ -57598,11 +57652,11 @@
       </c>
       <c r="B70" s="16">
         <f t="shared" si="14"/>
-        <v>6.7762635780344032E+48</v>
+        <v>1.3552527156068806E+48</v>
       </c>
       <c r="C70" s="16">
         <f t="shared" si="19"/>
-        <v>5.5084155209524622E+41</v>
+        <v>1.1016831041904924E+41</v>
       </c>
       <c r="D70">
         <f t="shared" si="12"/>
@@ -57618,11 +57672,11 @@
       </c>
       <c r="M70" s="16">
         <f t="shared" si="16"/>
-        <v>2.032879073410321E+49</v>
+        <v>4.0657581468206419E+48</v>
       </c>
       <c r="N70" s="16">
         <f t="shared" si="17"/>
-        <v>8.1315162936412838E+48</v>
+        <v>1.6263032587282567E+48</v>
       </c>
       <c r="Q70">
         <f t="shared" si="20"/>
@@ -57636,11 +57690,11 @@
       </c>
       <c r="B71" s="16">
         <f t="shared" si="14"/>
-        <v>3.3881317890172016E+49</v>
+        <v>6.7762635780344032E+48</v>
       </c>
       <c r="C71" s="16">
         <f t="shared" si="19"/>
-        <v>2.5038252367965733E+42</v>
+        <v>5.0076504735931473E+41</v>
       </c>
       <c r="D71">
         <f t="shared" si="12"/>
@@ -57656,11 +57710,11 @@
       </c>
       <c r="M71" s="16">
         <f t="shared" si="16"/>
-        <v>1.0164395367051605E+50</v>
+        <v>2.032879073410321E+49</v>
       </c>
       <c r="N71" s="16">
         <f t="shared" si="17"/>
-        <v>4.0657581468206419E+49</v>
+        <v>8.1315162936412838E+48</v>
       </c>
       <c r="Q71">
         <f t="shared" si="20"/>
@@ -57674,11 +57728,11 @@
       </c>
       <c r="B72" s="16">
         <f t="shared" si="14"/>
-        <v>1.6940658945086007E+50</v>
+        <v>3.3881317890172016E+49</v>
       </c>
       <c r="C72" s="16">
         <f t="shared" si="19"/>
-        <v>1.1381023803620788E+43</v>
+        <v>2.2762047607241574E+42</v>
       </c>
       <c r="D72">
         <f t="shared" si="12"/>
@@ -57694,11 +57748,11 @@
       </c>
       <c r="M72" s="16">
         <f t="shared" si="16"/>
-        <v>5.0821976835258022E+50</v>
+        <v>1.0164395367051605E+50</v>
       </c>
       <c r="N72" s="16">
         <f t="shared" si="17"/>
-        <v>2.0328790734103206E+50</v>
+        <v>4.0657581468206419E+49</v>
       </c>
       <c r="Q72">
         <f t="shared" si="20"/>
@@ -57712,11 +57766,11 @@
       </c>
       <c r="B73" s="16">
         <f t="shared" si="14"/>
-        <v>8.4703294725430046E+50</v>
+        <v>1.6940658945086007E+50</v>
       </c>
       <c r="C73" s="16">
         <f t="shared" si="19"/>
-        <v>5.1731926380094488E+43</v>
+        <v>1.0346385276018897E+43</v>
       </c>
       <c r="D73">
         <f t="shared" si="12"/>
@@ -57732,11 +57786,11 @@
       </c>
       <c r="M73" s="16">
         <f t="shared" si="16"/>
-        <v>2.5410988417629014E+51</v>
+        <v>5.0821976835258022E+50</v>
       </c>
       <c r="N73" s="16">
         <f t="shared" si="17"/>
-        <v>1.0164395367051604E+51</v>
+        <v>2.0328790734103206E+50</v>
       </c>
       <c r="Q73">
         <f t="shared" si="20"/>
@@ -57750,11 +57804,11 @@
       </c>
       <c r="B74" s="16">
         <f t="shared" si="14"/>
-        <v>4.2351647362715023E+51</v>
+        <v>8.4703294725430046E+50</v>
       </c>
       <c r="C74" s="16">
         <f t="shared" si="19"/>
-        <v>2.3514511990952036E+44</v>
+        <v>4.7029023981904077E+43</v>
       </c>
       <c r="D74">
         <f t="shared" si="12"/>
@@ -57770,11 +57824,11 @@
       </c>
       <c r="M74" s="16">
         <f t="shared" si="16"/>
-        <v>1.2705494208814508E+52</v>
+        <v>2.5410988417629014E+51</v>
       </c>
       <c r="N74" s="16">
         <f t="shared" si="17"/>
-        <v>5.0821976835258027E+51</v>
+        <v>1.0164395367051604E+51</v>
       </c>
       <c r="Q74">
         <f t="shared" si="20"/>
@@ -57788,11 +57842,11 @@
       </c>
       <c r="B75" s="16">
         <f t="shared" si="14"/>
-        <v>2.117582368135751E+52</v>
+        <v>4.2351647362715023E+51</v>
       </c>
       <c r="C75" s="16">
         <f t="shared" si="19"/>
-        <v>1.0688414541341834E+45</v>
+        <v>2.1376829082683669E+44</v>
       </c>
       <c r="D75">
         <f t="shared" si="12"/>
@@ -57808,11 +57862,11 @@
       </c>
       <c r="M75" s="16">
         <f t="shared" si="16"/>
-        <v>6.3527471044072525E+52</v>
+        <v>1.2705494208814508E+52</v>
       </c>
       <c r="N75" s="16">
         <f t="shared" si="17"/>
-        <v>2.5410988417629011E+52</v>
+        <v>5.0821976835258027E+51</v>
       </c>
       <c r="Q75">
         <f t="shared" si="20"/>
@@ -57826,11 +57880,11 @@
       </c>
       <c r="B76" s="16">
         <f t="shared" si="14"/>
-        <v>1.0587911840678756E+53</v>
+        <v>2.117582368135751E+52</v>
       </c>
       <c r="C76" s="16">
         <f t="shared" si="19"/>
-        <v>4.8583702460644704E+45</v>
+        <v>9.7167404921289396E+44</v>
       </c>
       <c r="D76">
         <f t="shared" si="12"/>
@@ -57846,11 +57900,11 @@
       </c>
       <c r="M76" s="16">
         <f t="shared" si="16"/>
-        <v>3.1763735522036267E+53</v>
+        <v>6.3527471044072525E+52</v>
       </c>
       <c r="N76" s="16">
         <f t="shared" si="17"/>
-        <v>1.2705494208814507E+53</v>
+        <v>2.5410988417629011E+52</v>
       </c>
       <c r="Q76">
         <f t="shared" si="20"/>
@@ -57864,11 +57918,11 @@
       </c>
       <c r="B77" s="16">
         <f t="shared" si="14"/>
-        <v>5.2939559203393774E+53</v>
+        <v>1.0587911840678756E+53</v>
       </c>
       <c r="C77" s="16">
         <f t="shared" si="19"/>
-        <v>2.2083501118474859E+46</v>
+        <v>4.4167002236949727E+45</v>
       </c>
       <c r="D77">
         <f t="shared" si="12"/>
@@ -57884,11 +57938,11 @@
       </c>
       <c r="M77" s="16">
         <f t="shared" si="16"/>
-        <v>1.588186776101813E+54</v>
+        <v>3.1763735522036267E+53</v>
       </c>
       <c r="N77" s="16">
         <f t="shared" si="17"/>
-        <v>6.3527471044072525E+53</v>
+        <v>1.2705494208814507E+53</v>
       </c>
       <c r="Q77">
         <f t="shared" si="20"/>
@@ -57902,11 +57956,11 @@
       </c>
       <c r="B78" s="16">
         <f t="shared" si="14"/>
-        <v>2.6469779601696889E+54</v>
+        <v>5.2939559203393774E+53</v>
       </c>
       <c r="C78" s="16">
         <f t="shared" si="19"/>
-        <v>1.003795505385221E+47</v>
+        <v>2.0075910107704418E+46</v>
       </c>
       <c r="D78">
         <f t="shared" si="12"/>
@@ -57922,11 +57976,11 @@
       </c>
       <c r="M78" s="16">
         <f t="shared" si="16"/>
-        <v>7.9409338805090666E+54</v>
+        <v>1.588186776101813E+54</v>
       </c>
       <c r="N78" s="16">
         <f t="shared" si="17"/>
-        <v>3.1763735522036268E+54</v>
+        <v>6.3527471044072525E+53</v>
       </c>
       <c r="Q78">
         <f t="shared" si="20"/>
@@ -57940,11 +57994,11 @@
       </c>
       <c r="B79" s="16">
         <f t="shared" si="14"/>
-        <v>1.3234889800848446E+55</v>
+        <v>2.6469779601696889E+54</v>
       </c>
       <c r="C79" s="16">
         <f t="shared" si="19"/>
-        <v>4.5627068426600958E+47</v>
+        <v>9.1254136853201899E+46</v>
       </c>
       <c r="D79">
         <f t="shared" si="12"/>
@@ -57960,11 +58014,11 @@
       </c>
       <c r="M79" s="16">
         <f t="shared" si="16"/>
-        <v>3.9704669402545337E+55</v>
+        <v>7.9409338805090666E+54</v>
       </c>
       <c r="N79" s="16">
         <f t="shared" si="17"/>
-        <v>1.5881867761018133E+55</v>
+        <v>3.1763735522036268E+54</v>
       </c>
       <c r="Q79">
         <f t="shared" si="20"/>
@@ -57978,11 +58032,11 @@
       </c>
       <c r="B80" s="16">
         <f t="shared" si="14"/>
-        <v>6.6174449004242223E+55</v>
+        <v>1.3234889800848446E+55</v>
       </c>
       <c r="C80" s="16">
         <f t="shared" si="19"/>
-        <v>2.0739576557545883E+48</v>
+        <v>4.1479153115091775E+47</v>
       </c>
       <c r="D80">
         <f t="shared" si="12"/>
@@ -57998,11 +58052,11 @@
       </c>
       <c r="M80" s="16">
         <f t="shared" si="16"/>
-        <v>1.9852334701272667E+56</v>
+        <v>3.9704669402545337E+55</v>
       </c>
       <c r="N80" s="16">
         <f t="shared" si="17"/>
-        <v>7.9409338805090663E+55</v>
+        <v>1.5881867761018133E+55</v>
       </c>
       <c r="Q80">
         <f t="shared" si="20"/>
@@ -58016,11 +58070,11 @@
       </c>
       <c r="B81" s="16">
         <f t="shared" si="14"/>
-        <v>3.3087224502121111E+56</v>
+        <v>6.6174449004242223E+55</v>
       </c>
       <c r="C81" s="16">
         <f t="shared" si="19"/>
-        <v>9.4270802534299446E+48</v>
+        <v>1.8854160506859887E+48</v>
       </c>
       <c r="D81">
         <f t="shared" si="12"/>
@@ -58036,11 +58090,11 @@
       </c>
       <c r="M81" s="16">
         <f t="shared" si="16"/>
-        <v>9.9261673506363334E+56</v>
+        <v>1.9852334701272667E+56</v>
       </c>
       <c r="N81" s="16">
         <f t="shared" si="17"/>
-        <v>3.9704669402545334E+56</v>
+        <v>7.9409338805090663E+55</v>
       </c>
       <c r="Q81">
         <f t="shared" si="20"/>
@@ -58054,11 +58108,11 @@
       </c>
       <c r="B82" s="16">
         <f t="shared" si="14"/>
-        <v>1.6543612251060556E+57</v>
+        <v>3.3087224502121111E+56</v>
       </c>
       <c r="C82" s="16">
         <f t="shared" si="19"/>
-        <v>4.2850364788317935E+49</v>
+        <v>8.5700729576635865E+48</v>
       </c>
       <c r="D82">
         <f t="shared" si="12"/>
@@ -58074,11 +58128,11 @@
       </c>
       <c r="M82" s="16">
         <f t="shared" si="16"/>
-        <v>4.9630836753181667E+57</v>
+        <v>9.9261673506363334E+56</v>
       </c>
       <c r="N82" s="16">
         <f t="shared" si="17"/>
-        <v>1.9852334701272667E+57</v>
+        <v>3.9704669402545334E+56</v>
       </c>
       <c r="Q82">
         <f t="shared" si="20"/>
@@ -58092,11 +58146,11 @@
       </c>
       <c r="B83" s="16">
         <f t="shared" si="14"/>
-        <v>8.2718061255302778E+57</v>
+        <v>1.6543612251060556E+57</v>
       </c>
       <c r="C83" s="16">
         <f t="shared" si="19"/>
-        <v>1.9477438540144514E+50</v>
+        <v>3.8954877080289025E+49</v>
       </c>
       <c r="D83">
         <f t="shared" si="12"/>
@@ -58112,11 +58166,11 @@
       </c>
       <c r="M83" s="16">
         <f t="shared" si="16"/>
-        <v>2.4815418376590832E+58</v>
+        <v>4.9630836753181667E+57</v>
       </c>
       <c r="N83" s="16">
         <f t="shared" si="17"/>
-        <v>9.9261673506363334E+57</v>
+        <v>1.9852334701272667E+57</v>
       </c>
       <c r="Q83">
         <f t="shared" si="20"/>
@@ -58134,7 +58188,7 @@
   <dimension ref="A1:F83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -58166,7 +58220,7 @@
       <c r="F1" s="17"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="25" t="s">
         <v>41</v>
       </c>
       <c r="B2" s="20" t="str">
@@ -58193,7 +58247,7 @@
       </c>
       <c r="B3" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B3))</f>
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="C3" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C3))</f>
@@ -58201,11 +58255,11 @@
       </c>
       <c r="D3" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M3))</f>
-        <v>300</v>
+        <v>60</v>
       </c>
       <c r="E3" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N3))</f>
-        <v>120</v>
+        <v>24</v>
       </c>
       <c r="F3" s="17"/>
     </row>
@@ -58215,7 +58269,7 @@
       </c>
       <c r="B4" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B4))</f>
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="C4" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C4))</f>
@@ -58223,11 +58277,11 @@
       </c>
       <c r="D4" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M4))</f>
-        <v>1500</v>
+        <v>300</v>
       </c>
       <c r="E4" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N4))</f>
-        <v>600</v>
+        <v>120</v>
       </c>
       <c r="F4" s="17"/>
     </row>
@@ -58237,19 +58291,19 @@
       </c>
       <c r="B5" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B5))</f>
-        <v>2500</v>
+        <v>500</v>
       </c>
       <c r="C5" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C5))</f>
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="D5" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M5))</f>
-        <v>7500</v>
+        <v>1500</v>
       </c>
       <c r="E5" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N5))</f>
-        <v>3000</v>
+        <v>600</v>
       </c>
       <c r="F5" s="17"/>
     </row>
@@ -58259,19 +58313,19 @@
       </c>
       <c r="B6" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B6))</f>
-        <v>12500</v>
+        <v>2500</v>
       </c>
       <c r="C6" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C6))</f>
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="D6" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M6))</f>
-        <v>37500</v>
+        <v>7500</v>
       </c>
       <c r="E6" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N6))</f>
-        <v>15000</v>
+        <v>3000</v>
       </c>
       <c r="F6" s="17"/>
     </row>
@@ -58281,19 +58335,19 @@
       </c>
       <c r="B7" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B7))</f>
-        <v>62500</v>
+        <v>12500</v>
       </c>
       <c r="C7" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C7))</f>
-        <v>145</v>
+        <v>29</v>
       </c>
       <c r="D7" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M7))</f>
-        <v>187500</v>
+        <v>37500</v>
       </c>
       <c r="E7" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N7))</f>
-        <v>75000</v>
+        <v>15000</v>
       </c>
       <c r="F7" s="17"/>
     </row>
@@ -58303,19 +58357,19 @@
       </c>
       <c r="B8" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B8))</f>
-        <v>312500</v>
+        <v>62500</v>
       </c>
       <c r="C8" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C8))</f>
-        <v>362</v>
+        <v>73</v>
       </c>
       <c r="D8" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M8))</f>
-        <v>937500</v>
+        <v>187500</v>
       </c>
       <c r="E8" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N8))</f>
-        <v>375000</v>
+        <v>75000</v>
       </c>
       <c r="F8" s="17"/>
     </row>
@@ -58325,19 +58379,19 @@
       </c>
       <c r="B9" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B9))</f>
-        <v>1562500</v>
+        <v>312500</v>
       </c>
       <c r="C9" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C9))</f>
-        <v>905</v>
+        <v>181</v>
       </c>
       <c r="D9" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M9))</f>
-        <v>4687500</v>
+        <v>937500</v>
       </c>
       <c r="E9" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N9))</f>
-        <v>1875000</v>
+        <v>375000</v>
       </c>
       <c r="F9" s="17"/>
     </row>
@@ -58347,19 +58401,19 @@
       </c>
       <c r="B10" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B10))</f>
-        <v>7812500</v>
+        <v>1562500</v>
       </c>
       <c r="C10" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C10))</f>
-        <v>2261</v>
+        <v>453</v>
       </c>
       <c r="D10" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M10))</f>
-        <v>23437500</v>
+        <v>4687500</v>
       </c>
       <c r="E10" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N10))</f>
-        <v>9375000</v>
+        <v>1875000</v>
       </c>
       <c r="F10" s="17"/>
     </row>
@@ -58369,19 +58423,19 @@
       </c>
       <c r="B11" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B11))</f>
-        <v>39062500</v>
+        <v>7812500</v>
       </c>
       <c r="C11" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C11))</f>
-        <v>5652</v>
+        <v>1131</v>
       </c>
       <c r="D11" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M11))</f>
-        <v>117187500</v>
+        <v>23437500</v>
       </c>
       <c r="E11" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N11))</f>
-        <v>46875000</v>
+        <v>9375000</v>
       </c>
       <c r="F11" s="17"/>
     </row>
@@ -58391,19 +58445,19 @@
       </c>
       <c r="B12" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B12))</f>
-        <v>195312500</v>
+        <v>39062500</v>
       </c>
       <c r="C12" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C12))</f>
-        <v>18839</v>
+        <v>3768</v>
       </c>
       <c r="D12" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M12))</f>
-        <v>585937500</v>
+        <v>117187500</v>
       </c>
       <c r="E12" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N12))</f>
-        <v>234375000</v>
+        <v>46875000</v>
       </c>
       <c r="F12" s="17"/>
     </row>
@@ -58413,19 +58467,19 @@
       </c>
       <c r="B13" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B13))</f>
-        <v>976562500</v>
+        <v>195312500</v>
       </c>
       <c r="C13" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C13))</f>
-        <v>62794</v>
+        <v>12559</v>
       </c>
       <c r="D13" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M13))</f>
-        <v>2929687500</v>
+        <v>585937500</v>
       </c>
       <c r="E13" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N13))</f>
-        <v>1171875000</v>
+        <v>234375000</v>
       </c>
       <c r="F13" s="17"/>
     </row>
@@ -58435,19 +58489,19 @@
       </c>
       <c r="B14" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B14))</f>
-        <v>4882812500</v>
+        <v>976562500</v>
       </c>
       <c r="C14" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C14))</f>
-        <v>209312</v>
+        <v>41863</v>
       </c>
       <c r="D14" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M14))</f>
-        <v>14648437500</v>
+        <v>2929687500</v>
       </c>
       <c r="E14" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N14))</f>
-        <v>5859375000</v>
+        <v>1171875000</v>
       </c>
       <c r="F14" s="17"/>
     </row>
@@ -58457,19 +58511,19 @@
       </c>
       <c r="B15" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B15))</f>
-        <v>24414062500</v>
+        <v>4882812500</v>
       </c>
       <c r="C15" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C15))</f>
-        <v>697705</v>
+        <v>139541</v>
       </c>
       <c r="D15" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M15))</f>
-        <v>73242187500</v>
+        <v>14648437500</v>
       </c>
       <c r="E15" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N15))</f>
-        <v>29296875000</v>
+        <v>5859375000</v>
       </c>
       <c r="F15" s="17"/>
     </row>
@@ -58479,19 +58533,19 @@
       </c>
       <c r="B16" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B16))</f>
-        <v>122070312500</v>
+        <v>24414062500</v>
       </c>
       <c r="C16" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C16))</f>
-        <v>2325681</v>
+        <v>465137</v>
       </c>
       <c r="D16" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M16))</f>
-        <v>366210937500</v>
+        <v>73242187500</v>
       </c>
       <c r="E16" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N16))</f>
-        <v>146484375000</v>
+        <v>29296875000</v>
       </c>
       <c r="F16" s="17"/>
     </row>
@@ -58501,19 +58555,19 @@
       </c>
       <c r="B17" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B17))</f>
-        <v>610351562500</v>
+        <v>122070312500</v>
       </c>
       <c r="C17" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C17))</f>
-        <v>7752268</v>
+        <v>1550454</v>
       </c>
       <c r="D17" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M17))</f>
-        <v>1831054687500</v>
+        <v>366210937500</v>
       </c>
       <c r="E17" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N17))</f>
-        <v>732421875000</v>
+        <v>146484375000</v>
       </c>
       <c r="F17" s="17"/>
     </row>
@@ -58523,19 +58577,19 @@
       </c>
       <c r="B18" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B18))</f>
-        <v>3051757812500</v>
+        <v>610351562500</v>
       </c>
       <c r="C18" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C18))</f>
-        <v>35237582</v>
+        <v>7047517</v>
       </c>
       <c r="D18" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M18))</f>
-        <v>9155273437500</v>
+        <v>1831054687500</v>
       </c>
       <c r="E18" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N18))</f>
-        <v>3662109375000</v>
+        <v>732421875000</v>
       </c>
       <c r="F18" s="17"/>
     </row>
@@ -58545,19 +58599,19 @@
       </c>
       <c r="B19" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B19))</f>
-        <v>15258789062500</v>
+        <v>3051757812500</v>
       </c>
       <c r="C19" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C19))</f>
-        <v>160170827</v>
+        <v>32034166</v>
       </c>
       <c r="D19" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M19))</f>
-        <v>45776367187500</v>
+        <v>9155273437500</v>
       </c>
       <c r="E19" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N19))</f>
-        <v>18310546875000</v>
+        <v>3662109375000</v>
       </c>
       <c r="F19" s="17"/>
     </row>
@@ -58567,19 +58621,19 @@
       </c>
       <c r="B20" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B20))</f>
-        <v>76293945312500</v>
+        <v>15258789062500</v>
       </c>
       <c r="C20" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C20))</f>
-        <v>728049210</v>
+        <v>145609842</v>
       </c>
       <c r="D20" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M20))</f>
-        <v>228881835937500</v>
+        <v>45776367187500</v>
       </c>
       <c r="E20" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N20))</f>
-        <v>91552734375000</v>
+        <v>18310546875000</v>
       </c>
       <c r="F20" s="17"/>
     </row>
@@ -58589,19 +58643,19 @@
       </c>
       <c r="B21" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B21))</f>
-        <v>381469726562500</v>
+        <v>76293945312500</v>
       </c>
       <c r="C21" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C21))</f>
-        <v>3309314587</v>
+        <v>661862918</v>
       </c>
       <c r="D21" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M21))</f>
-        <v>1144409179687500</v>
+        <v>228881835937500</v>
       </c>
       <c r="E21" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N21))</f>
-        <v>457763671875000</v>
+        <v>91552734375000</v>
       </c>
       <c r="F21" s="17"/>
     </row>
@@ -58611,19 +58665,19 @@
       </c>
       <c r="B22" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B22))</f>
-        <v>1907348632812500</v>
+        <v>381469726562500</v>
       </c>
       <c r="C22" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C22))</f>
-        <v>15042339032</v>
+        <v>3008467807</v>
       </c>
       <c r="D22" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M22))</f>
-        <v>5722045898437500</v>
+        <v>1144409179687500</v>
       </c>
       <c r="E22" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N22))</f>
-        <v>2288818359375000</v>
+        <v>457763671875000</v>
       </c>
       <c r="F22" s="17"/>
     </row>
@@ -58633,19 +58687,19 @@
       </c>
       <c r="B23" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B23))</f>
-        <v>9536743164062500</v>
+        <v>1907348632812500</v>
       </c>
       <c r="C23" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C23))</f>
-        <v>68374268325</v>
+        <v>13674853665</v>
       </c>
       <c r="D23" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M23))</f>
-        <v>28610229492187500</v>
+        <v>5722045898437500</v>
       </c>
       <c r="E23" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N23))</f>
-        <v>11444091796875000</v>
+        <v>2288818359375000</v>
       </c>
       <c r="F23" s="17"/>
     </row>
@@ -58655,19 +58709,19 @@
       </c>
       <c r="B24" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B24))</f>
-        <v>47683715820312500</v>
+        <v>9536743164062500</v>
       </c>
       <c r="C24" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C24))</f>
-        <v>310792128749</v>
+        <v>62158425750</v>
       </c>
       <c r="D24" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M24))</f>
-        <v>143051147460937000</v>
+        <v>28610229492187500</v>
       </c>
       <c r="E24" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N24))</f>
-        <v>57220458984375000</v>
+        <v>11444091796875000</v>
       </c>
       <c r="F24" s="17"/>
     </row>
@@ -58677,19 +58731,19 @@
       </c>
       <c r="B25" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B25))</f>
-        <v>238418579101562000</v>
+        <v>47683715820312500</v>
       </c>
       <c r="C25" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C25))</f>
-        <v>1412691494310</v>
+        <v>282538298862</v>
       </c>
       <c r="D25" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M25))</f>
-        <v>715255737304687000</v>
+        <v>143051147460937000</v>
       </c>
       <c r="E25" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N25))</f>
-        <v>286102294921875000</v>
+        <v>57220458984375000</v>
       </c>
       <c r="F25" s="17"/>
     </row>
@@ -58699,19 +58753,19 @@
       </c>
       <c r="B26" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B26))</f>
-        <v>1192092895507810000</v>
+        <v>238418579101562000</v>
       </c>
       <c r="C26" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C26))</f>
-        <v>6421324974136</v>
+        <v>1284264994828</v>
       </c>
       <c r="D26" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M26))</f>
-        <v>3576278686523440000</v>
+        <v>715255737304687000</v>
       </c>
       <c r="E26" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N26))</f>
-        <v>1430511474609370000</v>
+        <v>286102294921875000</v>
       </c>
       <c r="F26" s="17"/>
     </row>
@@ -58721,19 +58775,19 @@
       </c>
       <c r="B27" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B27))</f>
-        <v>5960464477539060000</v>
+        <v>1192092895507810000</v>
       </c>
       <c r="C27" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C27))</f>
-        <v>29187840791525</v>
+        <v>5837568158305</v>
       </c>
       <c r="D27" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M27))</f>
-        <v>17881393432617200000</v>
+        <v>3576278686523440000</v>
       </c>
       <c r="E27" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N27))</f>
-        <v>7152557373046870000</v>
+        <v>1430511474609370000</v>
       </c>
       <c r="F27" s="17"/>
     </row>
@@ -58743,19 +58797,19 @@
       </c>
       <c r="B28" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B28))</f>
-        <v>29802322387695300000</v>
+        <v>5960464477539060000</v>
       </c>
       <c r="C28" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C28))</f>
-        <v>132672003597837</v>
+        <v>26534400719568</v>
       </c>
       <c r="D28" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M28))</f>
-        <v>89406967163085900000</v>
+        <v>17881393432617200000</v>
       </c>
       <c r="E28" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N28))</f>
-        <v>35762786865234400000</v>
+        <v>7152557373046870000</v>
       </c>
       <c r="F28" s="17"/>
     </row>
@@ -58765,19 +58819,19 @@
       </c>
       <c r="B29" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B29))</f>
-        <v>1.49011611938477E+20</v>
+        <v>29802322387695300000</v>
       </c>
       <c r="C29" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C29))</f>
-        <v>603054561808351</v>
+        <v>120610912361670</v>
       </c>
       <c r="D29" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M29))</f>
-        <v>4.4703483581543E+20</v>
+        <v>89406967163085900000</v>
       </c>
       <c r="E29" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N29))</f>
-        <v>1.78813934326172E+20</v>
+        <v>35762786865234400000</v>
       </c>
       <c r="F29" s="17"/>
     </row>
@@ -58787,19 +58841,19 @@
       </c>
       <c r="B30" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B30))</f>
-        <v>7.45058059692383E+20</v>
+        <v>1.49011611938477E+20</v>
       </c>
       <c r="C30" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C30))</f>
-        <v>2741157099128870</v>
+        <v>548231419825774</v>
       </c>
       <c r="D30" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M30))</f>
-        <v>2.23517417907715E+21</v>
+        <v>4.4703483581543E+20</v>
       </c>
       <c r="E30" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N30))</f>
-        <v>8.94069671630859E+20</v>
+        <v>1.78813934326172E+20</v>
       </c>
       <c r="F30" s="17"/>
     </row>
@@ -58809,19 +58863,19 @@
       </c>
       <c r="B31" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B31))</f>
-        <v>3.72529029846191E+21</v>
+        <v>7.45058059692383E+20</v>
       </c>
       <c r="C31" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C31))</f>
-        <v>12459804996040300</v>
+        <v>2491960999208060</v>
       </c>
       <c r="D31" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M31))</f>
-        <v>1.11758708953857E+22</v>
+        <v>2.23517417907715E+21</v>
       </c>
       <c r="E31" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N31))</f>
-        <v>4.4703483581543E+21</v>
+        <v>8.94069671630859E+20</v>
       </c>
       <c r="F31" s="17"/>
     </row>
@@ -58831,19 +58885,19 @@
       </c>
       <c r="B32" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B32))</f>
-        <v>1.86264514923096E+22</v>
+        <v>3.72529029846191E+21</v>
       </c>
       <c r="C32" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C32))</f>
-        <v>56635477254728700</v>
+        <v>11327095450945700</v>
       </c>
       <c r="D32" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M32))</f>
-        <v>5.58793544769287E+22</v>
+        <v>1.11758708953857E+22</v>
       </c>
       <c r="E32" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N32))</f>
-        <v>2.23517417907715E+22</v>
+        <v>4.4703483581543E+21</v>
       </c>
       <c r="F32" s="17"/>
     </row>
@@ -58853,19 +58907,19 @@
       </c>
       <c r="B33" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B33))</f>
-        <v>9.31322574615478E+22</v>
+        <v>1.86264514923096E+22</v>
       </c>
       <c r="C33" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C33))</f>
-        <v>257433987521494000</v>
+        <v>51486797504298800</v>
       </c>
       <c r="D33" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M33))</f>
-        <v>2.79396772384644E+23</v>
+        <v>5.58793544769287E+22</v>
       </c>
       <c r="E33" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N33))</f>
-        <v>1.11758708953857E+23</v>
+        <v>2.23517417907715E+22</v>
       </c>
       <c r="F33" s="17"/>
     </row>
@@ -58875,19 +58929,19 @@
       </c>
       <c r="B34" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B34))</f>
-        <v>4.65661287307739E+23</v>
+        <v>9.31322574615478E+22</v>
       </c>
       <c r="C34" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C34))</f>
-        <v>1170154488734060000</v>
+        <v>234030897746813000</v>
       </c>
       <c r="D34" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M34))</f>
-        <v>1.39698386192322E+24</v>
+        <v>2.79396772384644E+23</v>
       </c>
       <c r="E34" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N34))</f>
-        <v>5.58793544769287E+23</v>
+        <v>1.11758708953857E+23</v>
       </c>
       <c r="F34" s="17"/>
     </row>
@@ -58897,19 +58951,19 @@
       </c>
       <c r="B35" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B35))</f>
-        <v>2.3283064365387E+24</v>
+        <v>4.65661287307739E+23</v>
       </c>
       <c r="C35" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C35))</f>
-        <v>5318884039700290000</v>
+        <v>1063776807940060000</v>
       </c>
       <c r="D35" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M35))</f>
-        <v>6.98491930961609E+24</v>
+        <v>1.39698386192322E+24</v>
       </c>
       <c r="E35" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N35))</f>
-        <v>2.79396772384644E+24</v>
+        <v>5.58793544769287E+23</v>
       </c>
       <c r="F35" s="17"/>
     </row>
@@ -58919,19 +58973,19 @@
       </c>
       <c r="B36" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B36))</f>
-        <v>1.16415321826935E+25</v>
+        <v>2.3283064365387E+24</v>
       </c>
       <c r="C36" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C36))</f>
-        <v>24176745635001300000</v>
+        <v>4835349127000260000</v>
       </c>
       <c r="D36" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M36))</f>
-        <v>3.49245965480804E+25</v>
+        <v>6.98491930961609E+24</v>
       </c>
       <c r="E36" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N36))</f>
-        <v>1.39698386192322E+25</v>
+        <v>2.79396772384644E+24</v>
       </c>
       <c r="F36" s="17"/>
     </row>
@@ -58941,19 +58995,19 @@
       </c>
       <c r="B37" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B37))</f>
-        <v>5.82076609134674E+25</v>
+        <v>1.16415321826935E+25</v>
       </c>
       <c r="C37" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C37))</f>
-        <v>1.09894298340915E+20</v>
+        <v>21978859668183000000</v>
       </c>
       <c r="D37" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M37))</f>
-        <v>1.74622982740402E+26</v>
+        <v>3.49245965480804E+25</v>
       </c>
       <c r="E37" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N37))</f>
-        <v>6.98491930961609E+25</v>
+        <v>1.39698386192322E+25</v>
       </c>
       <c r="F37" s="17"/>
     </row>
@@ -58963,19 +59017,19 @@
       </c>
       <c r="B38" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B38))</f>
-        <v>2.91038304567337E+26</v>
+        <v>5.82076609134674E+25</v>
       </c>
       <c r="C38" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C38))</f>
-        <v>4.9951953791325E+20</v>
+        <v>99903907582650000000</v>
       </c>
       <c r="D38" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M38))</f>
-        <v>8.73114913702011E+26</v>
+        <v>1.74622982740402E+26</v>
       </c>
       <c r="E38" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N38))</f>
-        <v>3.49245965480804E+26</v>
+        <v>6.98491930961609E+25</v>
       </c>
       <c r="F38" s="17"/>
     </row>
@@ -58985,19 +59039,19 @@
       </c>
       <c r="B39" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B39))</f>
-        <v>1.45519152283668E+27</v>
+        <v>2.91038304567337E+26</v>
       </c>
       <c r="C39" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C39))</f>
-        <v>2.27054335415114E+21</v>
+        <v>4.54108670830227E+20</v>
       </c>
       <c r="D39" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M39))</f>
-        <v>4.36557456851005E+27</v>
+        <v>8.73114913702011E+26</v>
       </c>
       <c r="E39" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N39))</f>
-        <v>1.74622982740402E+27</v>
+        <v>3.49245965480804E+26</v>
       </c>
       <c r="F39" s="17"/>
     </row>
@@ -59007,19 +59061,19 @@
       </c>
       <c r="B40" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B40))</f>
-        <v>7.27595761418342E+27</v>
+        <v>1.45519152283668E+27</v>
       </c>
       <c r="C40" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C40))</f>
-        <v>1.03206516097779E+22</v>
+        <v>2.06413032195558E+21</v>
       </c>
       <c r="D40" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M40))</f>
-        <v>2.18278728425503E+28</v>
+        <v>4.36557456851005E+27</v>
       </c>
       <c r="E40" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N40))</f>
-        <v>8.73114913702011E+27</v>
+        <v>1.74622982740402E+27</v>
       </c>
       <c r="F40" s="17"/>
     </row>
@@ -59029,19 +59083,19 @@
       </c>
       <c r="B41" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B41))</f>
-        <v>3.63797880709171E+28</v>
+        <v>7.27595761418342E+27</v>
       </c>
       <c r="C41" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C41))</f>
-        <v>4.69120527717177E+22</v>
+        <v>9.38241055434353E+21</v>
       </c>
       <c r="D41" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M41))</f>
-        <v>1.09139364212751E+29</v>
+        <v>2.18278728425503E+28</v>
       </c>
       <c r="E41" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N41))</f>
-        <v>4.36557456851005E+28</v>
+        <v>8.73114913702011E+27</v>
       </c>
       <c r="F41" s="17"/>
     </row>
@@ -59051,19 +59105,19 @@
       </c>
       <c r="B42" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B42))</f>
-        <v>1.81898940354586E+29</v>
+        <v>3.63797880709171E+28</v>
       </c>
       <c r="C42" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C42))</f>
-        <v>2.13236603507808E+23</v>
+        <v>4.26473207015615E+22</v>
       </c>
       <c r="D42" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M42))</f>
-        <v>5.45696821063757E+29</v>
+        <v>1.09139364212751E+29</v>
       </c>
       <c r="E42" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N42))</f>
-        <v>2.18278728425503E+29</v>
+        <v>4.36557456851005E+28</v>
       </c>
       <c r="F42" s="17"/>
     </row>
@@ -59073,19 +59127,19 @@
       </c>
       <c r="B43" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B43))</f>
-        <v>9.09494701772928E+29</v>
+        <v>1.81898940354586E+29</v>
       </c>
       <c r="C43" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C43))</f>
-        <v>9.69257288671853E+23</v>
+        <v>1.9385145773437E+23</v>
       </c>
       <c r="D43" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M43))</f>
-        <v>2.72848410531878E+30</v>
+        <v>5.45696821063757E+29</v>
       </c>
       <c r="E43" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N43))</f>
-        <v>1.09139364212751E+30</v>
+        <v>2.18278728425503E+29</v>
       </c>
       <c r="F43" s="17"/>
     </row>
@@ -59095,19 +59149,19 @@
       </c>
       <c r="B44" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B44))</f>
-        <v>4.54747350886464E+30</v>
+        <v>9.09494701772928E+29</v>
       </c>
       <c r="C44" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C44))</f>
-        <v>4.40571494850842E+24</v>
+        <v>8.81142989701684E+23</v>
       </c>
       <c r="D44" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M44))</f>
-        <v>1.36424205265939E+31</v>
+        <v>2.72848410531878E+30</v>
       </c>
       <c r="E44" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N44))</f>
-        <v>5.45696821063757E+30</v>
+        <v>1.09139364212751E+30</v>
       </c>
       <c r="F44" s="17"/>
     </row>
@@ -59117,19 +59171,19 @@
       </c>
       <c r="B45" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B45))</f>
-        <v>2.27373675443232E+31</v>
+        <v>4.54747350886464E+30</v>
       </c>
       <c r="C45" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C45))</f>
-        <v>2.00259770386746E+25</v>
+        <v>4.00519540773493E+24</v>
       </c>
       <c r="D45" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M45))</f>
-        <v>6.82121026329696E+31</v>
+        <v>1.36424205265939E+31</v>
       </c>
       <c r="E45" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N45))</f>
-        <v>2.72848410531878E+31</v>
+        <v>5.45696821063757E+30</v>
       </c>
       <c r="F45" s="17"/>
     </row>
@@ -59139,19 +59193,19 @@
       </c>
       <c r="B46" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B46))</f>
-        <v>1.13686837721616E+32</v>
+        <v>2.27373675443232E+31</v>
       </c>
       <c r="C46" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C46))</f>
-        <v>9.1027168357612E+25</v>
+        <v>1.82054336715224E+25</v>
       </c>
       <c r="D46" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M46))</f>
-        <v>3.41060513164848E+32</v>
+        <v>6.82121026329696E+31</v>
       </c>
       <c r="E46" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N46))</f>
-        <v>1.36424205265939E+32</v>
+        <v>2.72848410531878E+31</v>
       </c>
       <c r="F46" s="17"/>
     </row>
@@ -59161,19 +59215,19 @@
       </c>
       <c r="B47" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B47))</f>
-        <v>5.6843418860808E+32</v>
+        <v>1.13686837721616E+32</v>
       </c>
       <c r="C47" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C47))</f>
-        <v>4.13759856170963E+26</v>
+        <v>8.27519712341927E+25</v>
       </c>
       <c r="D47" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M47))</f>
-        <v>1.70530256582424E+33</v>
+        <v>3.41060513164848E+32</v>
       </c>
       <c r="E47" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N47))</f>
-        <v>6.82121026329696E+32</v>
+        <v>1.36424205265939E+32</v>
       </c>
       <c r="F47" s="17"/>
     </row>
@@ -59183,19 +59237,19 @@
       </c>
       <c r="B48" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B48))</f>
-        <v>2.8421709430404E+33</v>
+        <v>5.6843418860808E+32</v>
       </c>
       <c r="C48" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C48))</f>
-        <v>1.88072661895892E+27</v>
+        <v>3.76145323791785E+26</v>
       </c>
       <c r="D48" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M48))</f>
-        <v>8.5265128291212E+33</v>
+        <v>1.70530256582424E+33</v>
       </c>
       <c r="E48" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N48))</f>
-        <v>3.41060513164848E+33</v>
+        <v>6.82121026329696E+32</v>
       </c>
       <c r="F48" s="17"/>
     </row>
@@ -59205,19 +59259,19 @@
       </c>
       <c r="B49" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B49))</f>
-        <v>1.4210854715202E+34</v>
+        <v>2.8421709430404E+33</v>
       </c>
       <c r="C49" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C49))</f>
-        <v>8.5487573589042E+27</v>
+        <v>1.70975147178084E+27</v>
       </c>
       <c r="D49" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M49))</f>
-        <v>4.2632564145606E+34</v>
+        <v>8.5265128291212E+33</v>
       </c>
       <c r="E49" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N49))</f>
-        <v>1.70530256582424E+34</v>
+        <v>3.41060513164848E+33</v>
       </c>
       <c r="F49" s="17"/>
     </row>
@@ -59227,19 +59281,19 @@
       </c>
       <c r="B50" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B50))</f>
-        <v>7.105427357601E+34</v>
+        <v>1.4210854715202E+34</v>
       </c>
       <c r="C50" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C50))</f>
-        <v>3.88579879950191E+28</v>
+        <v>7.77159759900382E+27</v>
       </c>
       <c r="D50" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M50))</f>
-        <v>2.1316282072803E+35</v>
+        <v>4.2632564145606E+34</v>
       </c>
       <c r="E50" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N50))</f>
-        <v>8.5265128291212E+34</v>
+        <v>1.70530256582424E+34</v>
       </c>
       <c r="F50" s="17"/>
     </row>
@@ -59249,19 +59303,19 @@
       </c>
       <c r="B51" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B51))</f>
-        <v>3.5527136788005E+35</v>
+        <v>7.105427357601E+34</v>
       </c>
       <c r="C51" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C51))</f>
-        <v>1.76627218159178E+29</v>
+        <v>3.53254436318355E+28</v>
       </c>
       <c r="D51" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M51))</f>
-        <v>1.06581410364015E+36</v>
+        <v>2.1316282072803E+35</v>
       </c>
       <c r="E51" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N51))</f>
-        <v>4.2632564145606E+35</v>
+        <v>8.5265128291212E+34</v>
       </c>
       <c r="F51" s="17"/>
     </row>
@@ -59271,19 +59325,19 @@
       </c>
       <c r="B52" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B52))</f>
-        <v>1.77635683940025E+36</v>
+        <v>3.5527136788005E+35</v>
       </c>
       <c r="C52" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C52))</f>
-        <v>8.02850991632626E+29</v>
+        <v>1.60570198326525E+29</v>
       </c>
       <c r="D52" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M52))</f>
-        <v>5.32907051820075E+36</v>
+        <v>1.06581410364015E+36</v>
       </c>
       <c r="E52" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N52))</f>
-        <v>2.1316282072803E+36</v>
+        <v>4.2632564145606E+35</v>
       </c>
       <c r="F52" s="17"/>
     </row>
@@ -59293,19 +59347,19 @@
       </c>
       <c r="B53" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B53))</f>
-        <v>8.88178419700125E+36</v>
+        <v>1.77635683940025E+36</v>
       </c>
       <c r="C53" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C53))</f>
-        <v>3.64932268923921E+30</v>
+        <v>7.29864537847842E+29</v>
       </c>
       <c r="D53" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M53))</f>
-        <v>2.66453525910038E+37</v>
+        <v>5.32907051820075E+36</v>
       </c>
       <c r="E53" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N53))</f>
-        <v>1.06581410364015E+37</v>
+        <v>2.1316282072803E+36</v>
       </c>
       <c r="F53" s="17"/>
     </row>
@@ -59315,19 +59369,19 @@
       </c>
       <c r="B54" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B54))</f>
-        <v>4.44089209850063E+37</v>
+        <v>8.88178419700125E+36</v>
       </c>
       <c r="C54" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C54))</f>
-        <v>1.65878304056328E+31</v>
+        <v>3.31756608112655E+30</v>
       </c>
       <c r="D54" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M54))</f>
-        <v>1.33226762955019E+38</v>
+        <v>2.66453525910038E+37</v>
       </c>
       <c r="E54" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N54))</f>
-        <v>5.32907051820075E+37</v>
+        <v>1.06581410364015E+37</v>
       </c>
       <c r="F54" s="17"/>
     </row>
@@ -59337,19 +59391,19 @@
       </c>
       <c r="B55" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B55))</f>
-        <v>2.22044604925031E+38</v>
+        <v>4.44089209850063E+37</v>
       </c>
       <c r="C55" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C55))</f>
-        <v>7.53992291165125E+31</v>
+        <v>1.50798458233025E+31</v>
       </c>
       <c r="D55" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M55))</f>
-        <v>6.66133814775094E+38</v>
+        <v>1.33226762955019E+38</v>
       </c>
       <c r="E55" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N55))</f>
-        <v>2.66453525910038E+38</v>
+        <v>5.32907051820075E+37</v>
       </c>
       <c r="F55" s="17"/>
     </row>
@@ -59359,19 +59413,19 @@
       </c>
       <c r="B56" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B56))</f>
-        <v>1.11022302462516E+39</v>
+        <v>2.22044604925031E+38</v>
       </c>
       <c r="C56" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C56))</f>
-        <v>3.42723768711421E+32</v>
+        <v>6.85447537422841E+31</v>
       </c>
       <c r="D56" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M56))</f>
-        <v>3.33066907387547E+39</v>
+        <v>6.66133814775094E+38</v>
       </c>
       <c r="E56" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N56))</f>
-        <v>1.33226762955019E+39</v>
+        <v>2.66453525910038E+38</v>
       </c>
       <c r="F56" s="17"/>
     </row>
@@ -59381,19 +59435,19 @@
       </c>
       <c r="B57" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B57))</f>
-        <v>5.55111512312578E+39</v>
+        <v>1.11022302462516E+39</v>
       </c>
       <c r="C57" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C57))</f>
-        <v>1.55783531232464E+33</v>
+        <v>3.11567062464928E+32</v>
       </c>
       <c r="D57" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M57))</f>
-        <v>1.66533453693774E+40</v>
+        <v>3.33066907387547E+39</v>
       </c>
       <c r="E57" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N57))</f>
-        <v>6.66133814775094E+39</v>
+        <v>1.33226762955019E+39</v>
       </c>
       <c r="F57" s="17"/>
     </row>
@@ -59403,19 +59457,19 @@
       </c>
       <c r="B58" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B58))</f>
-        <v>2.77555756156289E+40</v>
+        <v>5.55111512312578E+39</v>
       </c>
       <c r="C58" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C58))</f>
-        <v>7.08106960147563E+33</v>
+        <v>1.41621392029513E+33</v>
       </c>
       <c r="D58" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M58))</f>
-        <v>8.32667268468867E+40</v>
+        <v>1.66533453693774E+40</v>
       </c>
       <c r="E58" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N58))</f>
-        <v>3.33066907387547E+40</v>
+        <v>6.66133814775094E+39</v>
       </c>
       <c r="F58" s="17"/>
     </row>
@@ -59425,19 +59479,19 @@
       </c>
       <c r="B59" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B59))</f>
-        <v>1.38777878078145E+41</v>
+        <v>2.77555756156289E+40</v>
       </c>
       <c r="C59" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C59))</f>
-        <v>3.21866800067074E+34</v>
+        <v>6.43733600134148E+33</v>
       </c>
       <c r="D59" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M59))</f>
-        <v>4.16333634234434E+41</v>
+        <v>8.32667268468867E+40</v>
       </c>
       <c r="E59" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N59))</f>
-        <v>1.66533453693773E+41</v>
+        <v>3.33066907387547E+40</v>
       </c>
       <c r="F59" s="17"/>
     </row>
@@ -59447,19 +59501,19 @@
       </c>
       <c r="B60" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B60))</f>
-        <v>6.93889390390723E+41</v>
+        <v>1.38777878078145E+41</v>
       </c>
       <c r="C60" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C60))</f>
-        <v>1.46303090939579E+35</v>
+        <v>2.92606181879158E+34</v>
       </c>
       <c r="D60" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M60))</f>
-        <v>2.08166817117217E+42</v>
+        <v>4.16333634234434E+41</v>
       </c>
       <c r="E60" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N60))</f>
-        <v>8.32667268468867E+41</v>
+        <v>1.66533453693773E+41</v>
       </c>
       <c r="F60" s="17"/>
     </row>
@@ -59469,19 +59523,19 @@
       </c>
       <c r="B61" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B61))</f>
-        <v>3.46944695195361E+42</v>
+        <v>6.93889390390723E+41</v>
       </c>
       <c r="C61" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C61))</f>
-        <v>6.6501404972536E+35</v>
+        <v>1.33002809945072E+35</v>
       </c>
       <c r="D61" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M61))</f>
-        <v>1.04083408558608E+43</v>
+        <v>2.08166817117217E+42</v>
       </c>
       <c r="E61" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N61))</f>
-        <v>4.16333634234434E+42</v>
+        <v>8.32667268468867E+41</v>
       </c>
       <c r="F61" s="17"/>
     </row>
@@ -59491,19 +59545,19 @@
       </c>
       <c r="B62" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B62))</f>
-        <v>1.73472347597681E+43</v>
+        <v>3.46944695195361E+42</v>
       </c>
       <c r="C62" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C62))</f>
-        <v>3.02279113511527E+36</v>
+        <v>6.04558227023054E+35</v>
       </c>
       <c r="D62" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M62))</f>
-        <v>5.20417042793042E+43</v>
+        <v>1.04083408558608E+43</v>
       </c>
       <c r="E62" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N62))</f>
-        <v>2.08166817117217E+43</v>
+        <v>4.16333634234434E+42</v>
       </c>
       <c r="F62" s="17"/>
     </row>
@@ -59513,19 +59567,19 @@
       </c>
       <c r="B63" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B63))</f>
-        <v>8.67361737988404E+43</v>
+        <v>1.73472347597681E+43</v>
       </c>
       <c r="C63" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C63))</f>
-        <v>1.37399597050694E+37</v>
+        <v>2.74799194101388E+36</v>
       </c>
       <c r="D63" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M63))</f>
-        <v>2.60208521396521E+44</v>
+        <v>5.20417042793042E+43</v>
       </c>
       <c r="E63" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N63))</f>
-        <v>1.04083408558608E+44</v>
+        <v>2.08166817117217E+43</v>
       </c>
       <c r="F63" s="17"/>
     </row>
@@ -59535,19 +59589,19 @@
       </c>
       <c r="B64" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B64))</f>
-        <v>4.33680868994202E+44</v>
+        <v>8.67361737988404E+43</v>
       </c>
       <c r="C64" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C64))</f>
-        <v>6.24543622957701E+37</v>
+        <v>1.2490872459154E+37</v>
       </c>
       <c r="D64" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M64))</f>
-        <v>1.30104260698261E+45</v>
+        <v>2.60208521396521E+44</v>
       </c>
       <c r="E64" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N64))</f>
-        <v>5.20417042793042E+44</v>
+        <v>1.04083408558608E+44</v>
       </c>
       <c r="F64" s="17"/>
     </row>
@@ -59557,19 +59611,19 @@
       </c>
       <c r="B65" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B65))</f>
-        <v>2.16840434497101E+45</v>
+        <v>4.33680868994202E+44</v>
       </c>
       <c r="C65" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C65))</f>
-        <v>2.83883464980773E+38</v>
+        <v>5.67766929961546E+37</v>
       </c>
       <c r="D65" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M65))</f>
-        <v>6.50521303491303E+45</v>
+        <v>1.30104260698261E+45</v>
       </c>
       <c r="E65" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N65))</f>
-        <v>2.60208521396521E+45</v>
+        <v>5.20417042793042E+44</v>
       </c>
       <c r="F65" s="17"/>
     </row>
@@ -59579,19 +59633,19 @@
       </c>
       <c r="B66" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B66))</f>
-        <v>1.0842021724855E+46</v>
+        <v>2.16840434497101E+45</v>
       </c>
       <c r="C66" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C66))</f>
-        <v>1.29037938627624E+39</v>
+        <v>2.58075877255248E+38</v>
       </c>
       <c r="D66" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M66))</f>
-        <v>3.25260651745651E+46</v>
+        <v>6.50521303491303E+45</v>
       </c>
       <c r="E66" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N66))</f>
-        <v>1.30104260698261E+46</v>
+        <v>2.60208521396521E+45</v>
       </c>
       <c r="F66" s="17"/>
     </row>
@@ -59601,19 +59655,19 @@
       </c>
       <c r="B67" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B67))</f>
-        <v>5.42101086242752E+46</v>
+        <v>1.0842021724855E+46</v>
       </c>
       <c r="C67" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C67))</f>
-        <v>5.86536084671018E+39</v>
+        <v>1.17307216934204E+39</v>
       </c>
       <c r="D67" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M67))</f>
-        <v>1.62630325872826E+47</v>
+        <v>3.25260651745651E+46</v>
       </c>
       <c r="E67" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N67))</f>
-        <v>6.50521303491303E+46</v>
+        <v>1.30104260698261E+46</v>
       </c>
       <c r="F67" s="17"/>
     </row>
@@ -59623,19 +59677,19 @@
       </c>
       <c r="B68" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B68))</f>
-        <v>2.71050543121376E+47</v>
+        <v>5.42101086242752E+46</v>
       </c>
       <c r="C68" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C68))</f>
-        <v>2.66607311214099E+40</v>
+        <v>5.33214622428198E+39</v>
       </c>
       <c r="D68" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M68))</f>
-        <v>8.13151629364129E+47</v>
+        <v>1.62630325872826E+47</v>
       </c>
       <c r="E68" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N68))</f>
-        <v>3.25260651745651E+47</v>
+        <v>6.50521303491303E+46</v>
       </c>
       <c r="F68" s="17"/>
     </row>
@@ -59645,19 +59699,19 @@
       </c>
       <c r="B69" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B69))</f>
-        <v>1.35525271560688E+48</v>
+        <v>2.71050543121376E+47</v>
       </c>
       <c r="C69" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C69))</f>
-        <v>1.21185141460954E+41</v>
+        <v>2.42370282921908E+40</v>
       </c>
       <c r="D69" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M69))</f>
-        <v>4.06575814682064E+48</v>
+        <v>8.13151629364129E+47</v>
       </c>
       <c r="E69" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N69))</f>
-        <v>1.62630325872826E+48</v>
+        <v>3.25260651745651E+47</v>
       </c>
       <c r="F69" s="17"/>
     </row>
@@ -59667,19 +59721,19 @@
       </c>
       <c r="B70" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B70))</f>
-        <v>6.7762635780344E+48</v>
+        <v>1.35525271560688E+48</v>
       </c>
       <c r="C70" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C70))</f>
-        <v>5.50841552095246E+41</v>
+        <v>1.10168310419049E+41</v>
       </c>
       <c r="D70" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M70))</f>
-        <v>2.03287907341032E+49</v>
+        <v>4.06575814682064E+48</v>
       </c>
       <c r="E70" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N70))</f>
-        <v>8.13151629364128E+48</v>
+        <v>1.62630325872826E+48</v>
       </c>
       <c r="F70" s="17"/>
     </row>
@@ -59689,19 +59743,19 @@
       </c>
       <c r="B71" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B71))</f>
-        <v>3.3881317890172E+49</v>
+        <v>6.7762635780344E+48</v>
       </c>
       <c r="C71" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C71))</f>
-        <v>2.50382523679657E+42</v>
+        <v>5.00765047359315E+41</v>
       </c>
       <c r="D71" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M71))</f>
-        <v>1.01643953670516E+50</v>
+        <v>2.03287907341032E+49</v>
       </c>
       <c r="E71" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N71))</f>
-        <v>4.06575814682064E+49</v>
+        <v>8.13151629364128E+48</v>
       </c>
       <c r="F71" s="17"/>
     </row>
@@ -59711,19 +59765,19 @@
       </c>
       <c r="B72" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B72))</f>
-        <v>1.6940658945086E+50</v>
+        <v>3.3881317890172E+49</v>
       </c>
       <c r="C72" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C72))</f>
-        <v>1.13810238036208E+43</v>
+        <v>2.27620476072416E+42</v>
       </c>
       <c r="D72" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M72))</f>
-        <v>5.0821976835258E+50</v>
+        <v>1.01643953670516E+50</v>
       </c>
       <c r="E72" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N72))</f>
-        <v>2.03287907341032E+50</v>
+        <v>4.06575814682064E+49</v>
       </c>
       <c r="F72" s="17"/>
     </row>
@@ -59733,19 +59787,19 @@
       </c>
       <c r="B73" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B73))</f>
-        <v>8.470329472543E+50</v>
+        <v>1.6940658945086E+50</v>
       </c>
       <c r="C73" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C73))</f>
-        <v>5.17319263800945E+43</v>
+        <v>1.03463852760189E+43</v>
       </c>
       <c r="D73" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M73))</f>
-        <v>2.5410988417629E+51</v>
+        <v>5.0821976835258E+50</v>
       </c>
       <c r="E73" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N73))</f>
-        <v>1.01643953670516E+51</v>
+        <v>2.03287907341032E+50</v>
       </c>
       <c r="F73" s="17"/>
     </row>
@@ -59755,19 +59809,19 @@
       </c>
       <c r="B74" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B74))</f>
-        <v>4.2351647362715E+51</v>
+        <v>8.470329472543E+50</v>
       </c>
       <c r="C74" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C74))</f>
-        <v>2.3514511990952E+44</v>
+        <v>4.70290239819041E+43</v>
       </c>
       <c r="D74" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M74))</f>
-        <v>1.27054942088145E+52</v>
+        <v>2.5410988417629E+51</v>
       </c>
       <c r="E74" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N74))</f>
-        <v>5.0821976835258E+51</v>
+        <v>1.01643953670516E+51</v>
       </c>
       <c r="F74" s="17"/>
     </row>
@@ -59777,19 +59831,19 @@
       </c>
       <c r="B75" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B75))</f>
-        <v>2.11758236813575E+52</v>
+        <v>4.2351647362715E+51</v>
       </c>
       <c r="C75" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C75))</f>
-        <v>1.06884145413418E+45</v>
+        <v>2.13768290826837E+44</v>
       </c>
       <c r="D75" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M75))</f>
-        <v>6.35274710440725E+52</v>
+        <v>1.27054942088145E+52</v>
       </c>
       <c r="E75" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N75))</f>
-        <v>2.5410988417629E+52</v>
+        <v>5.0821976835258E+51</v>
       </c>
       <c r="F75" s="17"/>
     </row>
@@ -59799,19 +59853,19 @@
       </c>
       <c r="B76" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B76))</f>
-        <v>1.05879118406788E+53</v>
+        <v>2.11758236813575E+52</v>
       </c>
       <c r="C76" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C76))</f>
-        <v>4.85837024606447E+45</v>
+        <v>9.71674049212894E+44</v>
       </c>
       <c r="D76" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M76))</f>
-        <v>3.17637355220363E+53</v>
+        <v>6.35274710440725E+52</v>
       </c>
       <c r="E76" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N76))</f>
-        <v>1.27054942088145E+53</v>
+        <v>2.5410988417629E+52</v>
       </c>
       <c r="F76" s="17"/>
     </row>
@@ -59821,19 +59875,19 @@
       </c>
       <c r="B77" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B77))</f>
-        <v>5.29395592033938E+53</v>
+        <v>1.05879118406788E+53</v>
       </c>
       <c r="C77" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C77))</f>
-        <v>2.20835011184749E+46</v>
+        <v>4.41670022369497E+45</v>
       </c>
       <c r="D77" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M77))</f>
-        <v>1.58818677610181E+54</v>
+        <v>3.17637355220363E+53</v>
       </c>
       <c r="E77" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N77))</f>
-        <v>6.35274710440725E+53</v>
+        <v>1.27054942088145E+53</v>
       </c>
       <c r="F77" s="17"/>
     </row>
@@ -59843,19 +59897,19 @@
       </c>
       <c r="B78" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B78))</f>
-        <v>2.64697796016969E+54</v>
+        <v>5.29395592033938E+53</v>
       </c>
       <c r="C78" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C78))</f>
-        <v>1.00379550538522E+47</v>
+        <v>2.00759101077044E+46</v>
       </c>
       <c r="D78" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M78))</f>
-        <v>7.94093388050907E+54</v>
+        <v>1.58818677610181E+54</v>
       </c>
       <c r="E78" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N78))</f>
-        <v>3.17637355220363E+54</v>
+        <v>6.35274710440725E+53</v>
       </c>
       <c r="F78" s="17"/>
     </row>
@@ -59865,19 +59919,19 @@
       </c>
       <c r="B79" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B79))</f>
-        <v>1.32348898008484E+55</v>
+        <v>2.64697796016969E+54</v>
       </c>
       <c r="C79" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C79))</f>
-        <v>4.5627068426601E+47</v>
+        <v>9.12541368532019E+46</v>
       </c>
       <c r="D79" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M79))</f>
-        <v>3.97046694025453E+55</v>
+        <v>7.94093388050907E+54</v>
       </c>
       <c r="E79" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N79))</f>
-        <v>1.58818677610181E+55</v>
+        <v>3.17637355220363E+54</v>
       </c>
       <c r="F79" s="17"/>
     </row>
@@ -59887,19 +59941,19 @@
       </c>
       <c r="B80" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B80))</f>
-        <v>6.61744490042422E+55</v>
+        <v>1.32348898008484E+55</v>
       </c>
       <c r="C80" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C80))</f>
-        <v>2.07395765575459E+48</v>
+        <v>4.14791531150918E+47</v>
       </c>
       <c r="D80" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M80))</f>
-        <v>1.98523347012727E+56</v>
+        <v>3.97046694025453E+55</v>
       </c>
       <c r="E80" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N80))</f>
-        <v>7.94093388050907E+55</v>
+        <v>1.58818677610181E+55</v>
       </c>
       <c r="F80" s="17"/>
     </row>
@@ -59909,19 +59963,19 @@
       </c>
       <c r="B81" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B81))</f>
-        <v>3.30872245021211E+56</v>
+        <v>6.61744490042422E+55</v>
       </c>
       <c r="C81" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C81))</f>
-        <v>9.42708025342994E+48</v>
+        <v>1.88541605068599E+48</v>
       </c>
       <c r="D81" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M81))</f>
-        <v>9.92616735063633E+56</v>
+        <v>1.98523347012727E+56</v>
       </c>
       <c r="E81" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N81))</f>
-        <v>3.97046694025453E+56</v>
+        <v>7.94093388050907E+55</v>
       </c>
       <c r="F81" s="17"/>
     </row>
@@ -59931,19 +59985,19 @@
       </c>
       <c r="B82" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B82))</f>
-        <v>1.65436122510606E+57</v>
+        <v>3.30872245021211E+56</v>
       </c>
       <c r="C82" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C82))</f>
-        <v>4.28503647883179E+49</v>
+        <v>8.57007295766359E+48</v>
       </c>
       <c r="D82" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M82))</f>
-        <v>4.96308367531817E+57</v>
+        <v>9.92616735063633E+56</v>
       </c>
       <c r="E82" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N82))</f>
-        <v>1.98523347012727E+57</v>
+        <v>3.97046694025453E+56</v>
       </c>
       <c r="F82" s="17"/>
     </row>
@@ -59953,19 +60007,19 @@
       </c>
       <c r="B83" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!B83))</f>
-        <v>8.27180612553028E+57</v>
+        <v>1.65436122510606E+57</v>
       </c>
       <c r="C83" s="20" t="str">
         <f>TRIM(_xlfn.CEILING.MATH( TownCenterIncome!C83))</f>
-        <v>1.94774385401445E+50</v>
+        <v>3.8954877080289E+49</v>
       </c>
       <c r="D83" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH( TownCenterIncome!M83))</f>
-        <v>2.48154183765908E+58</v>
+        <v>4.96308367531817E+57</v>
       </c>
       <c r="E83" s="20" t="str">
         <f>TRIM(_xlfn.FLOOR.MATH(TownCenterIncome!N83))</f>
-        <v>9.92616735063633E+57</v>
+        <v>1.98523347012727E+57</v>
       </c>
       <c r="F83" s="17"/>
     </row>

</xml_diff>